<commit_message>
Ultimo excel de socios y empresas
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Socios.xlsx
+++ b/MyProject2/Content/Excels/Socios.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23713"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44845782-672A-4D52-A2D5-346B65CD1C20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF564D2D-1F63-4807-89FB-8CD8A09079AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registro de usuarios" sheetId="1" r:id="rId1"/>
+    <sheet name="Registro de empresas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -26,14 +27,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Nomre y apellidos</t>
   </si>
   <si>
-    <t>Username</t>
-  </si>
-  <si>
     <t>Empresa</t>
   </si>
   <si>
@@ -46,16 +44,55 @@
     <t>PW Generado</t>
   </si>
   <si>
-    <t>Alfonso Gutierres Palomares</t>
-  </si>
-  <si>
-    <t>Alfonsi</t>
+    <t>Goberto Calleja Calleja</t>
   </si>
   <si>
     <t>Secpho</t>
   </si>
   <si>
-    <t>alfonsi@gmail.com</t>
+    <t>user1@gmail.com</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>Victor Gonzales</t>
+  </si>
+  <si>
+    <t>VicG@gmail.com</t>
+  </si>
+  <si>
+    <t>Daniel Carvajal</t>
+  </si>
+  <si>
+    <t>Inventado</t>
+  </si>
+  <si>
+    <t>danic@gmail.com</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>Tipo De Entidad</t>
+  </si>
+  <si>
+    <t>Actividad</t>
+  </si>
+  <si>
+    <t>Dirección</t>
+  </si>
+  <si>
+    <t>Contacto</t>
+  </si>
+  <si>
+    <t>Logo Url</t>
   </si>
 </sst>
 </file>
@@ -433,22 +470,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="3" max="4" width="20.28515625" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,28 +501,97 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>12345</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{C2F86D22-9865-448C-9AA4-CDC742F80EAF}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{C2F86D22-9865-448C-9AA4-CDC742F80EAF}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{8CBFEC48-6B8B-4800-A873-F9E52DC933FF}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{357FAB8B-B79A-4589-8ED4-3EB9E5D199AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACD1D1C-4031-4818-B1E7-AE253C20CE05}">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="A1:H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
excel Get Last Row
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Socios.xlsx
+++ b/MyProject2/Content/Excels/Socios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\Secpholand\MyProject2\Content\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A927CC-13A9-4FAC-9A9B-CAEA82C9D031}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B24DF9D-05E0-4314-AE58-767A78D00946}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registro de usuarios" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>Nomre y apellidos</t>
   </si>
@@ -47,9 +47,6 @@
     <t>user1@gmail.com</t>
   </si>
   <si>
-    <t>user1</t>
-  </si>
-  <si>
     <t>Victor Gonzales</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>Descripción</t>
   </si>
   <si>
-    <t>Url</t>
-  </si>
-  <si>
     <t>Tipo De Entidad</t>
   </si>
   <si>
@@ -89,16 +83,100 @@
     <t>Logo Url</t>
   </si>
   <si>
-    <t>Creada?</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
     <t>Cargo</t>
+  </si>
+  <si>
+    <t>Centro de I+D+i</t>
+  </si>
+  <si>
+    <t>Grupo de Investigación de Universidad</t>
+  </si>
+  <si>
+    <t>Desarrollo de software</t>
+  </si>
+  <si>
+    <t>Fabricante de componentes</t>
+  </si>
+  <si>
+    <t>Fabricante de módulos</t>
+  </si>
+  <si>
+    <t>Fabricante de sistemas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingeniería </t>
+  </si>
+  <si>
+    <t>Distribución de productos</t>
+  </si>
+  <si>
+    <t>Consultoría de I+D+i</t>
+  </si>
+  <si>
+    <t>startup</t>
+  </si>
+  <si>
+    <t>Aceleradora</t>
+  </si>
+  <si>
+    <t>Incubadora</t>
+  </si>
+  <si>
+    <t>Venture capital</t>
+  </si>
+  <si>
+    <t>Business Angel</t>
+  </si>
+  <si>
+    <t>Corporate</t>
+  </si>
+  <si>
+    <t>Empresa industrial usuaria de tecnología</t>
+  </si>
+  <si>
+    <t>Hospital o centro sanitario</t>
+  </si>
+  <si>
+    <t>Medio de comunicación</t>
+  </si>
+  <si>
+    <t>Empresa de servicios</t>
+  </si>
+  <si>
+    <t>Administración pública</t>
+  </si>
+  <si>
+    <t>Tipos de empresas</t>
+  </si>
+  <si>
+    <t>valor</t>
+  </si>
+  <si>
+    <t>Url web</t>
+  </si>
+  <si>
+    <t>Creada? (no rellenar)</t>
+  </si>
+  <si>
+    <t>sdaf</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>sdf</t>
+  </si>
+  <si>
+    <t>dsf</t>
+  </si>
+  <si>
+    <t>sadf</t>
+  </si>
+  <si>
+    <t>adsf</t>
+  </si>
+  <si>
+    <t>dsaf</t>
   </si>
 </sst>
 </file>
@@ -478,8 +556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +574,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -522,32 +600,38 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2">
-        <v>12345</v>
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -562,72 +646,273 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACD1D1C-4031-4818-B1E7-AE253C20CE05}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="1" max="1" width="31" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" customWidth="1"/>
+    <col min="6" max="6" width="51" customWidth="1"/>
+    <col min="7" max="7" width="39.42578125" customWidth="1"/>
+    <col min="8" max="8" width="32" customWidth="1"/>
     <col min="9" max="9" width="26.42578125" customWidth="1"/>
+    <col min="13" max="13" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
       <c r="D2">
         <v>1</v>
       </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" t="s">
+        <v>48</v>
+      </c>
       <c r="I2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
       <c r="D3">
         <v>2</v>
       </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" t="s">
+        <v>45</v>
+      </c>
       <c r="I3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="M3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>46</v>
+      </c>
+      <c r="M4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D5">
         <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>49</v>
+      </c>
+      <c r="M6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>31</v>
+      </c>
+      <c r="N12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>32</v>
+      </c>
+      <c r="N13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>33</v>
+      </c>
+      <c r="N14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>34</v>
+      </c>
+      <c r="N15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>35</v>
+      </c>
+      <c r="N16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>36</v>
+      </c>
+      <c r="N17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>37</v>
+      </c>
+      <c r="N18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>38</v>
+      </c>
+      <c r="N19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>39</v>
+      </c>
+      <c r="N20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>40</v>
+      </c>
+      <c r="N21">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Registro de usuarios de excel
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Socios.xlsx
+++ b/MyProject2/Content/Excels/Socios.xlsx
@@ -1,31 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23716"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\Secpholand\MyProject2\Content\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B24DF9D-05E0-4314-AE58-767A78D00946}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{33E68AEC-8FFA-4AF0-AC94-7457FECFBF68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registro de usuarios" sheetId="1" r:id="rId1"/>
     <sheet name="Registro de empresas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="54">
   <si>
     <t>Nomre y apellidos</t>
   </si>
   <si>
+    <t>Cargo</t>
+  </si>
+  <si>
     <t>Empresa</t>
   </si>
   <si>
@@ -41,21 +55,33 @@
     <t>Goberto Calleja Calleja</t>
   </si>
   <si>
+    <t>CEO</t>
+  </si>
+  <si>
     <t>Secpho</t>
   </si>
   <si>
     <t>user1@gmail.com</t>
   </si>
   <si>
+    <t>user1</t>
+  </si>
+  <si>
     <t>Victor Gonzales</t>
   </si>
   <si>
+    <t>Administrador</t>
+  </si>
+  <si>
     <t>VicG@gmail.com</t>
   </si>
   <si>
     <t>Daniel Carvajal</t>
   </si>
   <si>
+    <t>Programador</t>
+  </si>
+  <si>
     <t>Inventado</t>
   </si>
   <si>
@@ -68,6 +94,9 @@
     <t>Descripción</t>
   </si>
   <si>
+    <t>Url web</t>
+  </si>
+  <si>
     <t>Tipo De Entidad</t>
   </si>
   <si>
@@ -83,15 +112,36 @@
     <t>Logo Url</t>
   </si>
   <si>
-    <t>Cargo</t>
+    <t>Creada? (no rellenar)</t>
+  </si>
+  <si>
+    <t>Tipos de empresas</t>
+  </si>
+  <si>
+    <t>valor</t>
+  </si>
+  <si>
+    <t>sdaf</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>dsf</t>
+  </si>
+  <si>
+    <t>sadf</t>
+  </si>
+  <si>
+    <t>Grupo de Investigación de Universidad</t>
+  </si>
+  <si>
+    <t>sdf</t>
   </si>
   <si>
     <t>Centro de I+D+i</t>
   </si>
   <si>
-    <t>Grupo de Investigación de Universidad</t>
-  </si>
-  <si>
     <t>Desarrollo de software</t>
   </si>
   <si>
@@ -144,46 +194,13 @@
   </si>
   <si>
     <t>Administración pública</t>
-  </si>
-  <si>
-    <t>Tipos de empresas</t>
-  </si>
-  <si>
-    <t>valor</t>
-  </si>
-  <si>
-    <t>Url web</t>
-  </si>
-  <si>
-    <t>Creada? (no rellenar)</t>
-  </si>
-  <si>
-    <t>sdaf</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>sdf</t>
-  </si>
-  <si>
-    <t>dsf</t>
-  </si>
-  <si>
-    <t>sadf</t>
-  </si>
-  <si>
-    <t>adsf</t>
-  </si>
-  <si>
-    <t>dsaf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,7 +275,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -556,11 +573,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
@@ -569,69 +586,72 @@
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -648,11 +668,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACD1D1C-4031-4818-B1E7-AE253C20CE05}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="41.28515625" customWidth="1"/>
@@ -666,250 +686,250 @@
     <col min="13" max="13" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="C2" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="H2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="I2" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14">
       <c r="C3" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="M3" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="N3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14">
       <c r="D4">
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="M4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="N4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14">
       <c r="D5">
         <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="M5" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="N5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14">
       <c r="I6" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="M6" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="N6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="M7" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="N7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="M8" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="N8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="M9" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="N9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14">
       <c r="M10" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="N10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="M11" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="N11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="M12" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="N12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="M13" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="N13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14">
       <c r="M14" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="N14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14">
       <c r="M15" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="N15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14">
       <c r="M16" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="N16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="13:14">
       <c r="M17" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="N17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="13:14">
       <c r="M18" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="N18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="13:14">
       <c r="M19" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="N19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="13:14">
       <c r="M20" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="N20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="13:14">
       <c r="M21" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="N21">
         <v>19</v>

</xml_diff>

<commit_message>
Registro de empresa (No modificar el excel)
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Socios.xlsx
+++ b/MyProject2/Content/Excels/Socios.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\Secpholand\MyProject2\Content\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2289CE18-BF93-49BE-9EB5-CA0E81D60C04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4404BFB3-C76C-4FF8-B272-78D6273BD89D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registro de usuarios" sheetId="1" r:id="rId1"/>
     <sheet name="Registro de empresas" sheetId="2" r:id="rId2"/>
+    <sheet name="Lista desplegables" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028" calcCompleted="0" concurrentCalc="0"/>
   <extLst>
@@ -127,46 +128,46 @@
     <t>No modificar? (desmarcar para cambiar)</t>
   </si>
   <si>
+    <t>creada en local</t>
+  </si>
+  <si>
+    <t>www.google.es</t>
+  </si>
+  <si>
+    <t>Prueba</t>
+  </si>
+  <si>
+    <t>AV. Martinéz Nº18</t>
+  </si>
+  <si>
+    <t>inventado@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.andalucialab.org/wp-content/uploads/2020/02/INSERTAR_LOGO2-768x576.jpg</t>
+  </si>
+  <si>
+    <t>Fantasma</t>
+  </si>
+  <si>
+    <t>No existe en BBDD</t>
+  </si>
+  <si>
+    <t>Bajo el puente Chorreón 4</t>
+  </si>
+  <si>
+    <t>chancleta@gmail.com</t>
+  </si>
+  <si>
+    <t>https://images-platform.99static.com/EGp-dYkafgmlRVundPa5cpxW0PA=/500x500/top/smart/99designs-contests-attachments/57/57785/attachment_57785485</t>
+  </si>
+  <si>
     <t>Tipos de empresas</t>
   </si>
   <si>
     <t>valor</t>
   </si>
   <si>
-    <t>creada en local</t>
-  </si>
-  <si>
-    <t>www.google.es</t>
-  </si>
-  <si>
-    <t>Prueba</t>
-  </si>
-  <si>
-    <t>AV. Martinéz Nº18</t>
-  </si>
-  <si>
-    <t>inventado@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.andalucialab.org/wp-content/uploads/2020/02/INSERTAR_LOGO2-768x576.jpg</t>
-  </si>
-  <si>
     <t>Grupo de Investigación de Universidad</t>
-  </si>
-  <si>
-    <t>Fantasma</t>
-  </si>
-  <si>
-    <t>No existe en BBDD</t>
-  </si>
-  <si>
-    <t>Bajo el puente Chorreón 4</t>
-  </si>
-  <si>
-    <t>chancleta@gmail.com</t>
-  </si>
-  <si>
-    <t>https://images-platform.99static.com/EGp-dYkafgmlRVundPa5cpxW0PA=/500x500/top/smart/99designs-contests-attachments/57/57785/attachment_57785485</t>
   </si>
   <si>
     <t>Centro de I+D+i</t>
@@ -674,10 +675,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -694,7 +695,7 @@
     <col min="13" max="13" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -722,54 +723,42 @@
       <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D2">
         <v>9</v>
       </c>
       <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="B3" t="s">
         <v>38</v>
       </c>
-      <c r="M2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>41</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3">
         <v>9</v>
@@ -778,163 +767,13 @@
         <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="M4" t="s">
-        <v>46</v>
-      </c>
-      <c r="N4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="M5" t="s">
-        <v>47</v>
-      </c>
-      <c r="N5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="M6" t="s">
-        <v>48</v>
-      </c>
-      <c r="N6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="M7" t="s">
-        <v>49</v>
-      </c>
-      <c r="N7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="M8" t="s">
-        <v>50</v>
-      </c>
-      <c r="N8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="M9" t="s">
-        <v>51</v>
-      </c>
-      <c r="N9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="M10" t="s">
-        <v>52</v>
-      </c>
-      <c r="N10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="M11" t="s">
-        <v>53</v>
-      </c>
-      <c r="N11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="M12" t="s">
-        <v>54</v>
-      </c>
-      <c r="N12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14">
-      <c r="M13" t="s">
-        <v>55</v>
-      </c>
-      <c r="N13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14">
-      <c r="M14" t="s">
-        <v>56</v>
-      </c>
-      <c r="N14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="M15" t="s">
-        <v>57</v>
-      </c>
-      <c r="N15">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="M16" t="s">
-        <v>58</v>
-      </c>
-      <c r="N16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="13:14">
-      <c r="M17" t="s">
-        <v>59</v>
-      </c>
-      <c r="N17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="13:14">
-      <c r="M18" t="s">
-        <v>60</v>
-      </c>
-      <c r="N18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="13:14">
-      <c r="M19" t="s">
-        <v>61</v>
-      </c>
-      <c r="N19">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="13:14">
-      <c r="M20" t="s">
-        <v>62</v>
-      </c>
-      <c r="N20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="13:14">
-      <c r="M21" t="s">
-        <v>63</v>
-      </c>
-      <c r="N21">
-        <v>19</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -947,5 +786,203 @@
     <hyperlink ref="H3" r:id="rId6" xr:uid="{F14F2088-2CFF-482A-A3F5-D08313E70843}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada inválida" error="Seleccione un valor de la lista" promptTitle="Tipo de empresa" prompt="Seleccione un tipo de empresa" xr:uid="{6641CC2D-120E-4DAF-A947-2EE2CB102D58}">
+          <x14:formula1>
+            <xm:f>'Lista desplegables'!$B$2:$B$21</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FEAA92-2554-4FDA-8B4F-9784BD0832E9}">
+  <dimension ref="A1:B21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Enviar hoja de datos a los usuarios por emails
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Socios.xlsx
+++ b/MyProject2/Content/Excels/Socios.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23808"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\Secpholand\MyProject2\Content\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4896E026-56D5-47A5-97D4-36089E4BB2ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="Registro de usuarios" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
   <si>
     <t>Nomre y apellidos</t>
   </si>
@@ -42,6 +41,9 @@
     <t>PW Generado</t>
   </si>
   <si>
+    <t>Email enviado</t>
+  </si>
+  <si>
     <t>Goberto Calleja Calleja</t>
   </si>
   <si>
@@ -51,7 +53,10 @@
     <t>Secpho</t>
   </si>
   <si>
-    <t>user1@gmail.com</t>
+    <t>danitecno99@yopmail.com</t>
+  </si>
+  <si>
+    <t>user1</t>
   </si>
   <si>
     <t>Victor Gonzales</t>
@@ -60,7 +65,16 @@
     <t>Administrador</t>
   </si>
   <si>
-    <t>VicG@gmail.com</t>
+    <t>Inventado</t>
+  </si>
+  <si>
+    <t>xhaned_d318x@hexud.com</t>
+  </si>
+  <si>
+    <t>victorgonzales</t>
+  </si>
+  <si>
+    <t>mDNL1:O:f5Lu</t>
   </si>
   <si>
     <t>Daniel Carvajal</t>
@@ -69,10 +83,16 @@
     <t>Programador</t>
   </si>
   <si>
-    <t>Inventado</t>
-  </si>
-  <si>
-    <t>danic@gmail.com</t>
+    <t>Luna</t>
+  </si>
+  <si>
+    <t>danitecno86@gmail.com</t>
+  </si>
+  <si>
+    <t>danielcarvajal</t>
+  </si>
+  <si>
+    <t>h=MflH=bN&gt;r\</t>
   </si>
   <si>
     <t>Name</t>
@@ -102,30 +122,12 @@
     <t>No modificar? (desmarcar para cambiar)</t>
   </si>
   <si>
-    <t>creada en local</t>
+    <t>Ese toro enamorado de la luna</t>
   </si>
   <si>
     <t>www.google.es</t>
   </si>
   <si>
-    <t>Prueba</t>
-  </si>
-  <si>
-    <t>AV. Martinéz Nº18</t>
-  </si>
-  <si>
-    <t>inventado@gmail.com</t>
-  </si>
-  <si>
-    <t>https://www.andalucialab.org/wp-content/uploads/2020/02/INSERTAR_LOGO2-768x576.jpg</t>
-  </si>
-  <si>
-    <t>Fantasma</t>
-  </si>
-  <si>
-    <t>No existe en BBDD</t>
-  </si>
-  <si>
     <t>Bajo el puente Chorreón 4</t>
   </si>
   <si>
@@ -133,6 +135,24 @@
   </si>
   <si>
     <t>https://images-platform.99static.com/EGp-dYkafgmlRVundPa5cpxW0PA=/500x500/top/smart/99designs-contests-attachments/57/57785/attachment_57785485</t>
+  </si>
+  <si>
+    <t>Carrefour</t>
+  </si>
+  <si>
+    <t>3x2 los jueves</t>
+  </si>
+  <si>
+    <t>Almacén</t>
+  </si>
+  <si>
+    <t>Rio Abajo 6</t>
+  </si>
+  <si>
+    <t>carrefour@gmail.com</t>
+  </si>
+  <si>
+    <t>https://1000marcas.net/wp-content/uploads/2020/11/Carrefour-Logo-500x283.png</t>
   </si>
   <si>
     <t>Tipos de empresas</t>
@@ -207,8 +227,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,21 +282,18 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -544,23 +561,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.14062" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="4" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -579,68 +598,98 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>12345</v>
+      </c>
+      <c r="G2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.14062" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="41.28515625" customWidth="1"/>
@@ -654,44 +703,44 @@
     <col min="13" max="13" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D2">
         <v>9</v>
@@ -700,65 +749,59 @@
         <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D3">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="H2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="C3" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="H3" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="H2" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId5"/>
+    <hyperlink ref="H3" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada inválida" error="Seleccione un valor de la lista" promptTitle="Tipo de empresa" prompt="Seleccione un tipo de empresa" xr:uid="{00000000-0002-0000-0100-000000000000}">
-          <x14:formula1>
+      <x14:dataValidations count="1">
+        <x14:dataValidation allowBlank="1" error="Seleccione un valor de la lista" errorTitle="Entrada inválida" prompt="Seleccione un tipo de empresa" promptTitle="Tipo de empresa" showErrorMessage="1" showInputMessage="1" type="list">
+          <x14:formula1 xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
             <xm:f>'Lista desplegables'!$B$2:$B$21</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">D2:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -767,181 +810,181 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D1048576"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B9">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B11">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B13">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B14">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B15">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B16">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B17">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="B18">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="B19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B20">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B21">
         <v>19</v>

</xml_diff>

<commit_message>
Modificación registro de socios
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Socios.xlsx
+++ b/MyProject2/Content/Excels/Socios.xlsx
@@ -1,27 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23808"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23822"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\Secpholand\MyProject2\Content\Excels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\WindowsNoEditor\Secpholand_0.6.14_\MyProject2\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDC12CE8-5007-4197-8D73-2558433FD9F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
+    <workbookView xWindow="-29490" yWindow="3255" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registro de usuarios" sheetId="1" r:id="rId1"/>
     <sheet name="Registro de empresas" sheetId="2" r:id="rId2"/>
-    <sheet name="Lista desplegables" sheetId="3" r:id="rId3"/>
+    <sheet name="Listas y leyendas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" concurrentCalc="0"/>
+  <calcPr calcId="191028" calcCompleted="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="119">
   <si>
     <t>Nomre y apellidos</t>
   </si>
@@ -35,15 +47,24 @@
     <t>Mail</t>
   </si>
   <si>
+    <t>Perfil</t>
+  </si>
+  <si>
+    <t>Tecs</t>
+  </si>
+  <si>
+    <t>Sects</t>
+  </si>
+  <si>
+    <t>Ambitos</t>
+  </si>
+  <si>
     <t>Username Generado</t>
   </si>
   <si>
     <t>PW Generado</t>
   </si>
   <si>
-    <t>Email enviado</t>
-  </si>
-  <si>
     <t>Goberto Calleja Calleja</t>
   </si>
   <si>
@@ -56,7 +77,10 @@
     <t>danitecno99@yopmail.com</t>
   </si>
   <si>
-    <t>user1</t>
+    <t>1+2+3</t>
+  </si>
+  <si>
+    <t>2+3</t>
   </si>
   <si>
     <t>Victor Gonzales</t>
@@ -71,10 +95,7 @@
     <t>xhaned_d318x@hexud.com</t>
   </si>
   <si>
-    <t>victorgonzales</t>
-  </si>
-  <si>
-    <t>mDNL1:O:f5Lu</t>
+    <t>0+2+6</t>
   </si>
   <si>
     <t>Daniel Carvajal</t>
@@ -89,10 +110,7 @@
     <t>danitecno86@gmail.com</t>
   </si>
   <si>
-    <t>danielcarvajal</t>
-  </si>
-  <si>
-    <t>h=MflH=bN&gt;r\</t>
+    <t>3+5</t>
   </si>
   <si>
     <t>Name</t>
@@ -161,54 +179,207 @@
     <t>valor</t>
   </si>
   <si>
+    <t>Tipos de Perfil</t>
+  </si>
+  <si>
+    <t>Tecnologías</t>
+  </si>
+  <si>
+    <t>Sectores</t>
+  </si>
+  <si>
     <t>Grupo de Investigación de Universidad</t>
   </si>
   <si>
+    <t>Scientific investigation</t>
+  </si>
+  <si>
+    <t>Sensors and scanning and imaging systems</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Industria 4.0</t>
+  </si>
+  <si>
     <t>Centro de I+D+i</t>
   </si>
   <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Laser systems</t>
+  </si>
+  <si>
+    <t>Agri-food</t>
+  </si>
+  <si>
+    <t>Salud y bienestar</t>
+  </si>
+  <si>
     <t>Desarrollo de software</t>
   </si>
   <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>Communication systems, networks and data transmission</t>
+  </si>
+  <si>
+    <t>Cosmetics and aesthetics</t>
+  </si>
+  <si>
+    <t>Ciudades inteligentes</t>
+  </si>
+  <si>
     <t>Fabricante de componentes</t>
   </si>
   <si>
+    <t>Marketing and Communication</t>
+  </si>
+  <si>
+    <t>Artificial intelligence</t>
+  </si>
+  <si>
+    <t>Chemical industry</t>
+  </si>
+  <si>
+    <t>Seguridad alimentaria</t>
+  </si>
+  <si>
     <t>Fabricante de módulos</t>
   </si>
   <si>
+    <t>Investment</t>
+  </si>
+  <si>
+    <t>Advanced materials</t>
+  </si>
+  <si>
+    <t>Pharmacist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agricultura, bosques y océanos </t>
+  </si>
+  <si>
     <t>Fabricante de sistemas</t>
   </si>
   <si>
+    <t>Startup</t>
+  </si>
+  <si>
+    <t>quantum technologies</t>
+  </si>
+  <si>
+    <t>Automotive</t>
+  </si>
+  <si>
+    <t>Movilidad inteligente y sostenible</t>
+  </si>
+  <si>
     <t xml:space="preserve">Ingeniería </t>
   </si>
   <si>
+    <t>Administrative management</t>
+  </si>
+  <si>
+    <t>3d print</t>
+  </si>
+  <si>
+    <t>Railway</t>
+  </si>
+  <si>
+    <t>Energía segura, limpia y eficiente</t>
+  </si>
+  <si>
     <t>Distribución de productos</t>
   </si>
   <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Biotechnology</t>
+  </si>
+  <si>
+    <t>Aerospace</t>
+  </si>
+  <si>
+    <t>Acción climática y medio ambiente</t>
+  </si>
+  <si>
     <t>Consultoría de I+D+i</t>
   </si>
   <si>
+    <t>Nanotechnology</t>
+  </si>
+  <si>
+    <t>Industrial manufacturing</t>
+  </si>
+  <si>
+    <t>Comunicaciones seguras, defensa y seguridad</t>
+  </si>
+  <si>
     <t>startup</t>
   </si>
   <si>
+    <t>Blockchain</t>
+  </si>
+  <si>
+    <t>Environment and energy</t>
+  </si>
+  <si>
     <t>Aceleradora</t>
   </si>
   <si>
+    <t>Robotics and drones</t>
+  </si>
+  <si>
+    <t>Telecommunications and cybersecurity</t>
+  </si>
+  <si>
     <t>Incubadora</t>
   </si>
   <si>
+    <t>Videogame and software development</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
     <t>Venture capital</t>
   </si>
   <si>
+    <t>Photovoltaic Power Systems</t>
+  </si>
+  <si>
+    <t>Raw Materials</t>
+  </si>
+  <si>
     <t>Business Angel</t>
   </si>
   <si>
+    <t>Advanced lighting</t>
+  </si>
+  <si>
+    <t>Building</t>
+  </si>
+  <si>
     <t>Corporate</t>
   </si>
   <si>
+    <t>Screens, displays and image reproduction</t>
+  </si>
+  <si>
+    <t>Other sectors</t>
+  </si>
+  <si>
     <t>Empresa industrial usuaria de tecnología</t>
   </si>
   <si>
+    <t>Electronic systems</t>
+  </si>
+  <si>
     <t>Hospital o centro sanitario</t>
   </si>
   <si>
@@ -219,16 +390,13 @@
   </si>
   <si>
     <t>Administración pública</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,8 +420,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,8 +474,37 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF305496"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF548235"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC65911"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -275,19 +512,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1"/>
+    <cellStyle name="Salida" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -295,8 +570,251 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BF399AE-12AB-4FE7-B934-DA1F50A1EE81}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{56351748-3DE4-4017-8F4F-05209C9073C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12611100" y="0"/>
+          <a:ext cx="3181350" cy="3228975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBF7E67A-7AED-4BDD-B06B-359900C40F53}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{2BF399AE-12AB-4FE7-B934-DA1F50A1EE81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16325850" y="0"/>
+          <a:ext cx="3819525" cy="2076450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{552F94A7-0DCB-40EA-9074-2CE4162E7328}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{CBF7E67A-7AED-4BDD-B06B-359900C40F53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7734300" y="0"/>
+          <a:ext cx="4362450" cy="3429000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D33C1669-1968-4C61-9E61-D4F1BE62A9A3}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{552F94A7-0DCB-40EA-9074-2CE4162E7328}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4391025" y="0"/>
+          <a:ext cx="2828925" cy="1914525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11768D78-2DD4-46BF-8F62-1C0D59ABFB4C}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{D33C1669-1968-4C61-9E61-D4F1BE62A9A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="3324225" cy="4314825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -561,135 +1079,170 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14062" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="20.28515625" customWidth="1"/>
     <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="10" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="9" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2">
-        <v>12345</v>
-      </c>
-      <c r="G2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>19</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="14.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>66</v>
+        <v>24</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="12">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2FA78B4C-C81F-4F10-8722-E2C4410D47DB}">
+          <x14:formula1>
+            <xm:f>'Listas y leyendas'!$F$2:$F$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EDBA41E3-2CEF-4D89-9B00-E735CD64189E}">
+          <x14:formula1>
+            <xm:f>'Listas y leyendas'!$O$2:$O$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14062" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="41.28515625" customWidth="1"/>
@@ -705,103 +1258,103 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D2">
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D3">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="G2" r:id="rId2"/>
-    <hyperlink ref="H2" r:id="rId3"/>
-    <hyperlink ref="C3" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId5"/>
-    <hyperlink ref="H3" r:id="rId6"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="G2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="H2" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="G3" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="H3" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations count="1">
-        <x14:dataValidation allowBlank="1" error="Seleccione un valor de la lista" errorTitle="Entrada inválida" prompt="Seleccione un tipo de empresa" promptTitle="Tipo de empresa" showErrorMessage="1" showInputMessage="1" type="list">
-          <x14:formula1 xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-            <xm:f>'Lista desplegables'!$B$2:$B$21</xm:f>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada inválida" error="Seleccione un valor de la lista" promptTitle="Tipo de empresa" prompt="Seleccione un tipo de empresa" xr:uid="{00000000-0002-0000-0100-000000000000}">
+          <x14:formula1>
+            <xm:f>'Listas y leyendas'!$B$2:$B$21</xm:f>
           </x14:formula1>
-          <xm:sqref xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">D2:D1048576</xm:sqref>
+          <xm:sqref>D2:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -810,187 +1363,630 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="39.5703125" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" customWidth="1"/>
+    <col min="8" max="8" width="55.42578125" customWidth="1"/>
+    <col min="11" max="11" width="38.140625" customWidth="1"/>
+    <col min="14" max="14" width="45.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="1" spans="1:15" ht="15.75">
+      <c r="A1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B2">
+      <c r="B1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="5"/>
+      <c r="H1" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="5"/>
+      <c r="K1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75">
+      <c r="A2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3">
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0</v>
+      </c>
+      <c r="J2" s="5"/>
+      <c r="K2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.75">
+      <c r="A3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" s="3">
+        <v>1</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O3" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.75">
+      <c r="A4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="3">
+        <v>2</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="L4" s="3">
+        <v>2</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="O4" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75">
+      <c r="A5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="3">
+        <v>3</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="L5" s="3">
+        <v>3</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="O5" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75">
+      <c r="A6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="3">
+        <v>4</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I6" s="3">
+        <v>4</v>
+      </c>
+      <c r="J6" s="5"/>
+      <c r="K6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="L6" s="3">
+        <v>4</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="O6" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75">
+      <c r="A7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="3">
+        <v>5</v>
+      </c>
+      <c r="J7" s="5"/>
+      <c r="K7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L7" s="3">
+        <v>5</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="O7" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75">
+      <c r="A8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="3">
+        <v>6</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="I8" s="3">
+        <v>6</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="L8" s="3">
+        <v>6</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="O8" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75">
+      <c r="A9" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="3">
+        <v>7</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I9" s="3">
+        <v>7</v>
+      </c>
+      <c r="J9" s="5"/>
+      <c r="K9" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="L9" s="3">
+        <v>7</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="O9" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75">
+      <c r="A10" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11">
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="3">
+        <v>8</v>
+      </c>
+      <c r="J10" s="5"/>
+      <c r="K10" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="L10" s="3">
+        <v>8</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O10" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.75">
+      <c r="A11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B12">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I11" s="3">
+        <v>9</v>
+      </c>
+      <c r="J11" s="5"/>
+      <c r="K11" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="L11" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75">
+      <c r="A12" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B13">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I12" s="3">
+        <v>10</v>
+      </c>
+      <c r="J12" s="5"/>
+      <c r="K12" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L12" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75">
+      <c r="A13" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13" s="3">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" s="3">
+        <v>11</v>
+      </c>
+      <c r="J13" s="5"/>
+      <c r="K13" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L13" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75">
+      <c r="A14" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15">
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I14" s="3">
+        <v>12</v>
+      </c>
+      <c r="J14" s="5"/>
+      <c r="K14" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L14" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75">
+      <c r="A15" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16">
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="I15" s="3">
+        <v>13</v>
+      </c>
+      <c r="J15" s="5"/>
+      <c r="K15" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="L15" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75">
+      <c r="A16" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17">
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16" s="3">
+        <v>14</v>
+      </c>
+      <c r="J16" s="5"/>
+      <c r="K16" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="L16" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="15.75">
+      <c r="A17" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="3">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18">
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="I17" s="3">
+        <v>15</v>
+      </c>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+    </row>
+    <row r="18" spans="1:12" ht="15.75">
+      <c r="A18" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+    </row>
+    <row r="19" spans="1:12" ht="15.75">
+      <c r="A19" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="3">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20">
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+    </row>
+    <row r="20" spans="1:12" ht="15.75">
+      <c r="A20" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21">
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75">
+      <c r="A21" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" s="3">
         <v>19</v>
       </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update registro de empresas con Excel
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Socios.xlsx
+++ b/MyProject2/Content/Excels/Socios.xlsx
@@ -1,39 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23906"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan\Desktop\Secpholand_Win64_0.6.18_EXPERIMENTAL\MyProject2\Content\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F2CB56B-70F2-4EF4-963D-B25E7460865B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4965" yWindow="3750" windowWidth="28800" windowHeight="15435" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4965" yWindow="3750" windowWidth="28800" windowHeight="15435"/>
   </bookViews>
   <sheets>
     <sheet name="Registro de usuarios" sheetId="1" r:id="rId1"/>
     <sheet name="Registro de empresas" sheetId="2" r:id="rId2"/>
     <sheet name="Listas y leyendas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191028" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="461">
   <si>
     <t>Nomre y apellidos</t>
   </si>
@@ -1003,7 +991,7 @@
   </si>
   <si>
     <r>
-      <t>ALTER TECHNOLOGY</t>
+      <t xml:space="preserve">ALTER TECHNOLOGY</t>
     </r>
     <r>
       <rPr>
@@ -1012,7 +1000,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t> provide a single point of contact for all high reliability electronic component requirements, covering testing, engineering, procurement, storage, quality control, certification and consultancy. They bring services both for new-build equipment and also for managing component obsolescence issues in operational equipment. They have also extended their component capability into specialized equipment testing and EMC certification. The company in many markets including, but not limited to, Aerospace, Security, Transport, Emergency Services, Health &amp; Safety and Automotive.</t>
+      <t xml:space="preserve"> provide a single point of contact for all high reliability electronic component requirements, covering testing, engineering, procurement, storage, quality control, certification and consultancy. They bring services both for new-build equipment and also for managing component obsolescence issues in operational equipment. They have also extended their component capability into specialized equipment testing and EMC certification. The company in many markets including, but not limited to, Aerospace, Security, Transport, Emergency Services, Health &amp; Safety and Automotive.</t>
     </r>
   </si>
   <si>
@@ -1067,7 +1055,7 @@
   </si>
   <si>
     <r>
-      <t>AOTECH</t>
+      <t xml:space="preserve">AOTECH</t>
     </r>
     <r>
       <rPr>
@@ -1076,7 +1064,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>is a spin-off company from the University of the Basque Country whose mission is to apply customized photonic solutions to all kind of industrial processes. Currently, the two main areas of activity are aeronautics and food industry. In aeronautics, they are developing a system to monitor structural health monitoring of blades in turbines and compressors. Whereas in their second area, food industry, they are going to apply NIR spectroscopy sensors to different processes. AOTECH plans to expand this activities to other sectors such as energy, automotive, metallurgy chemistry or environment.</t>
+      <t xml:space="preserve">is a spin-off company from the University of the Basque Country whose mission is to apply customized photonic solutions to all kind of industrial processes. Currently, the two main areas of activity are aeronautics and food industry. In aeronautics, they are developing a system to monitor structural health monitoring of blades in turbines and compressors. Whereas in their second area, food industry, they are going to apply NIR spectroscopy sensors to different processes. AOTECH plans to expand this activities to other sectors such as energy, automotive, metallurgy chemistry or environment.</t>
     </r>
   </si>
   <si>
@@ -1090,7 +1078,7 @@
   </si>
   <si>
     <r>
-      <t>Aragon Photonics Labs.</t>
+      <t xml:space="preserve">Aragon Photonics Labs.</t>
     </r>
     <r>
       <rPr>
@@ -1099,7 +1087,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>is a manufacturer of advanced optical test &amp; measurement instrumentation and fiber optic distributed sensing equipment based on proprietary patents. With more than 10 years experience and operating in more than 20 countries, Aragon Photonics provides test &amp; measurement products to photonic R&amp;D centers, optical telecom component manufacturers and telecom operators (optical spectrum analysis, passive component characterization, polarization analysis and phase measurement) and distributed acoustic sensing turnkey solutions for transport, energy and security infrastructures.</t>
+      <t xml:space="preserve">is a manufacturer of advanced optical test &amp; measurement instrumentation and fiber optic distributed sensing equipment based on proprietary patents. With more than 10 years experience and operating in more than 20 countries, Aragon Photonics provides test &amp; measurement products to photonic R&amp;D centers, optical telecom component manufacturers and telecom operators (optical spectrum analysis, passive component characterization, polarization analysis and phase measurement) and distributed acoustic sensing turnkey solutions for transport, energy and security infrastructures.</t>
     </r>
   </si>
   <si>
@@ -1199,7 +1187,7 @@
   </si>
   <si>
     <r>
-      <t>ICFO</t>
+      <t xml:space="preserve">ICFO</t>
     </r>
     <r>
       <rPr>
@@ -1208,7 +1196,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>is a research centre devoted to the science and technologies of light with fundamental and applied research programs that address standing issues such as health, renewable energies, information technologies, security and industrial processes, among others.  The centre hosts 400 professionals including researchers and PhD students, and collaborates with a wide range of companies around the world.  In particular, ICFO’s Corporate Liaison Program includes more than 25 national and international industries and corporations. Likewise, the institute actively promotes the creation of spin-off companies by ICFO researchers.</t>
+      <t xml:space="preserve">is a research centre devoted to the science and technologies of light with fundamental and applied research programs that address standing issues such as health, renewable energies, information technologies, security and industrial processes, among others.  The centre hosts 400 professionals including researchers and PhD students, and collaborates with a wide range of companies around the world.  In particular, ICFO’s Corporate Liaison Program includes more than 25 national and international industries and corporations. Likewise, the institute actively promotes the creation of spin-off companies by ICFO researchers.</t>
     </r>
   </si>
   <si>
@@ -1279,7 +1267,7 @@
   </si>
   <si>
     <r>
-      <t>Tekniker</t>
+      <t xml:space="preserve">Tekniker</t>
     </r>
     <r>
       <rPr>
@@ -1288,7 +1276,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>is an independent research organization, whose main working focus is to improve manufacturing technologies, that includes all the situations that characterises a product life cycle, from conception and design, until the end of working life. Automotive parts, machine tools, mechanical capital goods, aerospace, chemical and petroleum products and industrial and consumer electronics are the most relevant sectors served by Tekniker.Tekniker likes to define itself as a Mechatronics, Manufacturing Technologies and Microtechnologies centre. It mainly specialises in: designing consumer and industrial products, solving problems relating to friction, wear and lubrication, incorporating information technologies and communications in the plant, high precision, miniaturisation and micro/nanotechnologies.</t>
+      <t xml:space="preserve">is an independent research organization, whose main working focus is to improve manufacturing technologies, that includes all the situations that characterises a product life cycle, from conception and design, until the end of working life. Automotive parts, machine tools, mechanical capital goods, aerospace, chemical and petroleum products and industrial and consumer electronics are the most relevant sectors served by Tekniker.Tekniker likes to define itself as a Mechatronics, Manufacturing Technologies and Microtechnologies centre. It mainly specialises in: designing consumer and industrial products, solving problems relating to friction, wear and lubrication, incorporating information technologies and communications in the plant, high precision, miniaturisation and micro/nanotechnologies.</t>
     </r>
   </si>
   <si>
@@ -1518,12 +1506,15 @@
   </si>
   <si>
     <t>Administración pública</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -1719,43 +1710,43 @@
   </cellStyleXfs>
   <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFill="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="2" applyFill="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="2" applyFill="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyFill="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFill="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFill="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFill="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1765,7 +1756,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFill="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1791,22 +1782,19 @@
     </xf>
   </cellXfs>
   <cellStyles count="7">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1"/>
+    <cellStyle name="Salida" xfId="2" builtinId="21"/>
     <cellStyle name="Bueno" xfId="3" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8"/>
-    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Incorrecto" xfId="6" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Salida" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2074,14 +2062,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14062" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
@@ -2518,7 +2506,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="75">
+    <row r="17" spans="1:10" ht="75">
       <c r="A17" s="13" t="s">
         <v>69</v>
       </c>
@@ -2544,7 +2532,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="45">
+    <row r="18" spans="1:10" ht="45">
       <c r="A18" s="13" t="s">
         <v>72</v>
       </c>
@@ -2570,7 +2558,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="60">
+    <row r="19" spans="1:10" ht="60">
       <c r="A19" s="13" t="s">
         <v>75</v>
       </c>
@@ -2596,7 +2584,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="45">
+    <row r="20" spans="1:10" ht="45">
       <c r="A20" s="13" t="s">
         <v>78</v>
       </c>
@@ -2622,7 +2610,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="30">
+    <row r="21" spans="1:10" ht="30">
       <c r="A21" s="13" t="s">
         <v>81</v>
       </c>
@@ -2648,7 +2636,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30">
+    <row r="22" spans="1:10" ht="30">
       <c r="A22" s="13" t="s">
         <v>84</v>
       </c>
@@ -2674,7 +2662,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:10">
       <c r="A23" s="13" t="s">
         <v>87</v>
       </c>
@@ -2700,7 +2688,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="30">
+    <row r="24" spans="1:10" ht="30">
       <c r="A24" s="13" t="s">
         <v>90</v>
       </c>
@@ -2726,7 +2714,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="45">
+    <row r="25" spans="1:10" ht="45">
       <c r="A25" s="13" t="s">
         <v>93</v>
       </c>
@@ -2752,7 +2740,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30">
+    <row r="26" spans="1:10" ht="30">
       <c r="A26" s="13" t="s">
         <v>97</v>
       </c>
@@ -2778,7 +2766,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="30">
+    <row r="27" spans="1:10" ht="30">
       <c r="A27" s="13" t="s">
         <v>100</v>
       </c>
@@ -2804,7 +2792,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="30">
+    <row r="28" spans="1:10" ht="30">
       <c r="A28" s="13" t="s">
         <v>103</v>
       </c>
@@ -2830,7 +2818,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="30">
+    <row r="29" spans="1:10" ht="30">
       <c r="A29" s="13" t="s">
         <v>106</v>
       </c>
@@ -2856,7 +2844,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="30">
+    <row r="30" spans="1:10" ht="30">
       <c r="A30" s="13" t="s">
         <v>109</v>
       </c>
@@ -2882,7 +2870,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:10">
       <c r="A31" s="13" t="s">
         <v>112</v>
       </c>
@@ -2908,7 +2896,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="45">
+    <row r="32" spans="1:10" ht="45">
       <c r="A32" s="13" t="s">
         <v>115</v>
       </c>
@@ -2934,7 +2922,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="45">
+    <row r="33" spans="1:10" ht="45">
       <c r="A33" s="13" t="s">
         <v>119</v>
       </c>
@@ -2960,7 +2948,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="30">
+    <row r="34" spans="1:10" ht="30">
       <c r="A34" s="13" t="s">
         <v>122</v>
       </c>
@@ -2986,7 +2974,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="30">
+    <row r="35" spans="1:10" ht="30">
       <c r="A35" s="13" t="s">
         <v>129</v>
       </c>
@@ -3012,7 +3000,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="30">
+    <row r="36" spans="1:10" ht="30">
       <c r="A36" s="13" t="s">
         <v>132</v>
       </c>
@@ -3038,7 +3026,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="30">
+    <row r="37" spans="1:10" ht="30">
       <c r="A37" s="13" t="s">
         <v>135</v>
       </c>
@@ -3064,7 +3052,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="30">
+    <row r="38" spans="1:10" ht="30">
       <c r="A38" s="13" t="s">
         <v>138</v>
       </c>
@@ -3090,7 +3078,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="30">
+    <row r="39" spans="1:10" ht="30">
       <c r="A39" s="13" t="s">
         <v>142</v>
       </c>
@@ -3116,7 +3104,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:10">
       <c r="A40" s="13" t="s">
         <v>145</v>
       </c>
@@ -3142,7 +3130,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:10">
       <c r="A41" s="13" t="s">
         <v>148</v>
       </c>
@@ -3168,7 +3156,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="30">
+    <row r="42" spans="1:10" ht="30">
       <c r="A42" s="13" t="s">
         <v>151</v>
       </c>
@@ -3194,7 +3182,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="30">
+    <row r="43" spans="1:10" ht="30">
       <c r="A43" s="13" t="s">
         <v>154</v>
       </c>
@@ -3220,7 +3208,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:10">
       <c r="A44" s="13" t="s">
         <v>157</v>
       </c>
@@ -3246,7 +3234,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:10">
       <c r="A45" s="13" t="s">
         <v>164</v>
       </c>
@@ -3272,7 +3260,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="30">
+    <row r="46" spans="1:10" ht="30">
       <c r="A46" s="13" t="s">
         <v>167</v>
       </c>
@@ -3298,7 +3286,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="30">
+    <row r="47" spans="1:10" ht="30">
       <c r="A47" s="13" t="s">
         <v>169</v>
       </c>
@@ -3324,7 +3312,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="30">
+    <row r="48" spans="1:10" ht="30">
       <c r="A48" s="13" t="s">
         <v>175</v>
       </c>
@@ -3350,7 +3338,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:10">
       <c r="A49" s="13" t="s">
         <v>178</v>
       </c>
@@ -3376,7 +3364,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="60">
+    <row r="50" spans="1:10" ht="60">
       <c r="A50" s="13" t="s">
         <v>185</v>
       </c>
@@ -3402,7 +3390,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="60">
+    <row r="51" spans="1:10" ht="60">
       <c r="A51" s="13" t="s">
         <v>189</v>
       </c>
@@ -3428,7 +3416,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="60">
+    <row r="52" spans="1:10" ht="60">
       <c r="A52" s="13" t="s">
         <v>196</v>
       </c>
@@ -3454,7 +3442,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="105">
+    <row r="53" spans="1:10" ht="105">
       <c r="A53" s="13" t="s">
         <v>199</v>
       </c>
@@ -3480,7 +3468,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="30">
+    <row r="54" spans="1:10" ht="30">
       <c r="A54" s="13" t="s">
         <v>206</v>
       </c>
@@ -3506,7 +3494,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="30">
+    <row r="55" spans="1:10" ht="30">
       <c r="A55" s="13" t="s">
         <v>213</v>
       </c>
@@ -3532,7 +3520,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="26.25">
+    <row r="56" spans="1:10" ht="26.25">
       <c r="A56" s="13" t="s">
         <v>216</v>
       </c>
@@ -3558,7 +3546,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="30">
+    <row r="57" spans="1:10" ht="30">
       <c r="A57" s="13" t="s">
         <v>218</v>
       </c>
@@ -3584,7 +3572,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:10">
       <c r="A58" s="13" t="s">
         <v>223</v>
       </c>
@@ -3610,7 +3598,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="30">
+    <row r="59" spans="1:10" ht="30">
       <c r="A59" s="13" t="s">
         <v>226</v>
       </c>
@@ -3636,7 +3624,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:10">
       <c r="A60" s="13" t="s">
         <v>229</v>
       </c>
@@ -3662,7 +3650,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:10">
       <c r="A61" s="13" t="s">
         <v>232</v>
       </c>
@@ -3688,7 +3676,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="60">
+    <row r="62" spans="1:10" ht="60">
       <c r="A62" s="13" t="s">
         <v>239</v>
       </c>
@@ -3714,7 +3702,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="45">
+    <row r="63" spans="1:10" ht="45">
       <c r="A63" s="13" t="s">
         <v>245</v>
       </c>
@@ -3740,7 +3728,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:10">
       <c r="A64" s="13" t="s">
         <v>248</v>
       </c>
@@ -3766,7 +3754,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:10">
       <c r="A65" s="13" t="s">
         <v>250</v>
       </c>
@@ -3792,7 +3780,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="45">
+    <row r="66" spans="1:10" ht="45">
       <c r="A66" s="13" t="s">
         <v>253</v>
       </c>
@@ -3818,7 +3806,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="30">
+    <row r="67" spans="1:10" ht="30">
       <c r="A67" s="13" t="s">
         <v>256</v>
       </c>
@@ -3844,7 +3832,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="30">
+    <row r="68" spans="1:10" ht="30">
       <c r="A68" s="13" t="s">
         <v>262</v>
       </c>
@@ -3870,7 +3858,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="30">
+    <row r="69" spans="1:10" ht="30">
       <c r="A69" s="13" t="s">
         <v>268</v>
       </c>
@@ -3896,7 +3884,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:10">
       <c r="A70" s="13" t="s">
         <v>271</v>
       </c>
@@ -3922,7 +3910,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="45">
+    <row r="71" spans="1:10" ht="45">
       <c r="A71" s="13" t="s">
         <v>274</v>
       </c>
@@ -3952,18 +3940,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
-          <x14:formula1>
+      <x14:dataValidations count="2">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+          <x14:formula1 xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
             <xm:f>'Listas y leyendas'!$F$2:$F$9</xm:f>
           </x14:formula1>
-          <xm:sqref>E72:E1048576 C2:C71</xm:sqref>
+          <xm:sqref xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">E72:E1048576 C2:C71</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
-          <x14:formula1>
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+          <x14:formula1 xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
             <xm:f>'Listas y leyendas'!$O$2:$O$10</xm:f>
           </x14:formula1>
-          <xm:sqref>H72:H1048576</xm:sqref>
+          <xm:sqref xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">H72:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3972,14 +3960,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="I2" sqref="I2:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14062" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="76.5703125" customWidth="1"/>
@@ -4047,6 +4035,9 @@
       <c r="H2" t="s">
         <v>291</v>
       </c>
+      <c r="I2" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="195">
       <c r="A3" t="s">
@@ -4073,6 +4064,9 @@
       <c r="H3" t="s">
         <v>295</v>
       </c>
+      <c r="I3" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="180">
       <c r="A4" t="s">
@@ -4099,6 +4093,9 @@
       <c r="H4" t="s">
         <v>299</v>
       </c>
+      <c r="I4" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="270">
       <c r="A5" t="s">
@@ -4125,6 +4122,9 @@
       <c r="H5" t="s">
         <v>303</v>
       </c>
+      <c r="I5" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="165">
       <c r="A6" t="s">
@@ -4151,6 +4151,9 @@
       <c r="H6" t="s">
         <v>307</v>
       </c>
+      <c r="I6" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="120">
       <c r="A7" t="s">
@@ -4177,6 +4180,9 @@
       <c r="H7" t="s">
         <v>311</v>
       </c>
+      <c r="I7" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="51.75">
       <c r="A8" t="s">
@@ -4203,6 +4209,9 @@
       <c r="H8" t="s">
         <v>315</v>
       </c>
+      <c r="I8" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="102.75">
       <c r="A9" t="s">
@@ -4229,6 +4238,9 @@
       <c r="H9" t="s">
         <v>319</v>
       </c>
+      <c r="I9" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="315">
       <c r="A10" t="s">
@@ -4255,6 +4267,9 @@
       <c r="H10" t="s">
         <v>323</v>
       </c>
+      <c r="I10" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="405">
       <c r="A11" t="s">
@@ -4281,6 +4296,9 @@
       <c r="H11" t="s">
         <v>327</v>
       </c>
+      <c r="I11" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="90">
       <c r="A12" t="s">
@@ -4307,6 +4325,9 @@
       <c r="H12" t="s">
         <v>331</v>
       </c>
+      <c r="I12" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="102.75">
       <c r="A13" t="s">
@@ -4333,6 +4354,9 @@
       <c r="H13" t="s">
         <v>335</v>
       </c>
+      <c r="I13" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="345">
       <c r="A14" t="s">
@@ -4359,6 +4383,9 @@
       <c r="H14" t="s">
         <v>339</v>
       </c>
+      <c r="I14" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="150">
       <c r="A15" t="s">
@@ -4385,6 +4412,9 @@
       <c r="H15" t="s">
         <v>343</v>
       </c>
+      <c r="I15" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="77.25">
       <c r="A16" t="s">
@@ -4411,8 +4441,11 @@
       <c r="H16" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="75">
+      <c r="I16" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="75">
       <c r="A17" t="s">
         <v>191</v>
       </c>
@@ -4437,8 +4470,11 @@
       <c r="H17" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="375">
+      <c r="I17" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="375">
       <c r="A18" t="s">
         <v>201</v>
       </c>
@@ -4463,8 +4499,11 @@
       <c r="H18" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="102.75">
+      <c r="I18" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="102.75">
       <c r="A19" t="s">
         <v>208</v>
       </c>
@@ -4489,8 +4528,11 @@
       <c r="H19" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="51" customHeight="1">
+      <c r="I19" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="51" customHeight="1">
       <c r="A20" t="s">
         <v>220</v>
       </c>
@@ -4515,8 +4557,11 @@
       <c r="H20" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="115.5">
+      <c r="I20" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="115.5">
       <c r="A21" t="s">
         <v>234</v>
       </c>
@@ -4541,8 +4586,11 @@
       <c r="H21" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="102.75">
+      <c r="I21" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="102.75">
       <c r="A22" t="s">
         <v>241</v>
       </c>
@@ -4567,8 +4615,11 @@
       <c r="H22" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="115.5">
+      <c r="I22" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="115.5">
       <c r="A23" t="s">
         <v>257</v>
       </c>
@@ -4593,8 +4644,11 @@
       <c r="H23" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="64.5">
+      <c r="I23" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="64.5">
       <c r="A24" t="s">
         <v>269</v>
       </c>
@@ -4619,8 +4673,11 @@
       <c r="H24" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="38.25">
+      <c r="I24" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="38.25">
       <c r="A25" t="s">
         <v>272</v>
       </c>
@@ -4645,8 +4702,11 @@
       <c r="H25" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="128.25">
+      <c r="I25" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="128.25">
       <c r="A26" t="s">
         <v>276</v>
       </c>
@@ -4671,38 +4731,41 @@
       <c r="H26" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="B27" s="20"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:9">
       <c r="B28" s="21"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:9">
       <c r="B29" s="21"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:9">
       <c r="B30" s="20"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:9">
       <c r="B31" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
-          <x14:formula1>
+      <x14:dataValidations count="2">
+        <x14:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
+          <x14:formula1 xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
             <xm:f>'Listas y leyendas'!$F$2:$F$9</xm:f>
           </x14:formula1>
-          <xm:sqref>A2</xm:sqref>
+          <xm:sqref xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">A2</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada inválida" error="Seleccione un valor de la lista" promptTitle="Tipo de empresa" prompt="Seleccione un tipo de empresa" xr:uid="{00000000-0002-0000-0100-000001000000}">
-          <x14:formula1>
+        <x14:dataValidation allowBlank="1" error="Seleccione un valor de la lista" errorTitle="Entrada inválida" prompt="Seleccione un tipo de empresa" promptTitle="Tipo de empresa" showErrorMessage="1" showInputMessage="1" type="list">
+          <x14:formula1 xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
             <xm:f>'Listas y leyendas'!$B$2:$B$21</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">D2:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4711,14 +4774,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14062" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39.5703125" customWidth="1"/>
     <col min="5" max="5" width="30.85546875" customWidth="1"/>
@@ -5239,7 +5302,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15.75">
+    <row r="17" spans="1:15" ht="15.75">
       <c r="A17" s="2" t="s">
         <v>454</v>
       </c>
@@ -5261,7 +5324,7 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:12" ht="15.75">
+    <row r="18" spans="1:15" ht="15.75">
       <c r="A18" s="2" t="s">
         <v>456</v>
       </c>
@@ -5279,7 +5342,7 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="15.75">
+    <row r="19" spans="1:15" ht="15.75">
       <c r="A19" s="2" t="s">
         <v>457</v>
       </c>
@@ -5297,7 +5360,7 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:12" ht="15.75">
+    <row r="20" spans="1:15" ht="15.75">
       <c r="A20" s="2" t="s">
         <v>458</v>
       </c>
@@ -5315,7 +5378,7 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75">
+    <row r="21" spans="1:15" ht="15.75">
       <c r="A21" s="2" t="s">
         <v>459</v>
       </c>

</xml_diff>

<commit_message>
Registro de usuario en eventos SU (Working)
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Socios.xlsx
+++ b/MyProject2/Content/Excels/Socios.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23911"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23921"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEFB28E2-D20F-4C55-9680-D2CAC9012687}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registro de usuarios" sheetId="1" r:id="rId1"/>
     <sheet name="Registro de empresas" sheetId="2" r:id="rId2"/>
-    <sheet name="Listas y leyendas" sheetId="3" r:id="rId3"/>
+    <sheet name="Registro a eventos" sheetId="4" r:id="rId3"/>
+    <sheet name="Listas y leyendas" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028" concurrentCalc="0"/>
+  <calcPr calcId="191028" calcCompleted="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="539">
   <si>
     <t>Nomre y apellidos</t>
   </si>
@@ -1210,7 +1223,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">ALTER TECHNOLOGY</t>
+      <t>ALTER TECHNOLOGY</t>
     </r>
     <r>
       <rPr>
@@ -1219,7 +1232,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> provide a single point of contact for all high reliability electronic component requirements, covering testing, engineering, procurement, storage, quality control, certification and consultancy. They bring services both for new-build equipment and also for managing component obsolescence issues in operational equipment. They have also extended their component capability into specialized equipment testing and EMC certification. The company in many markets including, but not limited to, Aerospace, Security, Transport, Emergency Services, Health &amp; Safety and Automotive.</t>
+      <t> provide a single point of contact for all high reliability electronic component requirements, covering testing, engineering, procurement, storage, quality control, certification and consultancy. They bring services both for new-build equipment and also for managing component obsolescence issues in operational equipment. They have also extended their component capability into specialized equipment testing and EMC certification. The company in many markets including, but not limited to, Aerospace, Security, Transport, Emergency Services, Health &amp; Safety and Automotive.</t>
     </r>
   </si>
   <si>
@@ -1274,7 +1287,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">AOTECH</t>
+      <t>AOTECH</t>
     </r>
     <r>
       <rPr>
@@ -1283,7 +1296,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">is a spin-off company from the University of the Basque Country whose mission is to apply customized photonic solutions to all kind of industrial processes. Currently, the two main areas of activity are aeronautics and food industry. In aeronautics, they are developing a system to monitor structural health monitoring of blades in turbines and compressors. Whereas in their second area, food industry, they are going to apply NIR spectroscopy sensors to different processes. AOTECH plans to expand this activities to other sectors such as energy, automotive, metallurgy chemistry or environment.</t>
+      <t>is a spin-off company from the University of the Basque Country whose mission is to apply customized photonic solutions to all kind of industrial processes. Currently, the two main areas of activity are aeronautics and food industry. In aeronautics, they are developing a system to monitor structural health monitoring of blades in turbines and compressors. Whereas in their second area, food industry, they are going to apply NIR spectroscopy sensors to different processes. AOTECH plans to expand this activities to other sectors such as energy, automotive, metallurgy chemistry or environment.</t>
     </r>
   </si>
   <si>
@@ -1297,7 +1310,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Aragon Photonics Labs.</t>
+      <t>Aragon Photonics Labs.</t>
     </r>
     <r>
       <rPr>
@@ -1306,7 +1319,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">is a manufacturer of advanced optical test &amp; measurement instrumentation and fiber optic distributed sensing equipment based on proprietary patents. With more than 10 years experience and operating in more than 20 countries, Aragon Photonics provides test &amp; measurement products to photonic R&amp;D centers, optical telecom component manufacturers and telecom operators (optical spectrum analysis, passive component characterization, polarization analysis and phase measurement) and distributed acoustic sensing turnkey solutions for transport, energy and security infrastructures.</t>
+      <t>is a manufacturer of advanced optical test &amp; measurement instrumentation and fiber optic distributed sensing equipment based on proprietary patents. With more than 10 years experience and operating in more than 20 countries, Aragon Photonics provides test &amp; measurement products to photonic R&amp;D centers, optical telecom component manufacturers and telecom operators (optical spectrum analysis, passive component characterization, polarization analysis and phase measurement) and distributed acoustic sensing turnkey solutions for transport, energy and security infrastructures.</t>
     </r>
   </si>
   <si>
@@ -1406,7 +1419,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">ICFO</t>
+      <t>ICFO</t>
     </r>
     <r>
       <rPr>
@@ -1415,7 +1428,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">is a research centre devoted to the science and technologies of light with fundamental and applied research programs that address standing issues such as health, renewable energies, information technologies, security and industrial processes, among others.  The centre hosts 400 professionals including researchers and PhD students, and collaborates with a wide range of companies around the world.  In particular, ICFO’s Corporate Liaison Program includes more than 25 national and international industries and corporations. Likewise, the institute actively promotes the creation of spin-off companies by ICFO researchers.</t>
+      <t>is a research centre devoted to the science and technologies of light with fundamental and applied research programs that address standing issues such as health, renewable energies, information technologies, security and industrial processes, among others.  The centre hosts 400 professionals including researchers and PhD students, and collaborates with a wide range of companies around the world.  In particular, ICFO’s Corporate Liaison Program includes more than 25 national and international industries and corporations. Likewise, the institute actively promotes the creation of spin-off companies by ICFO researchers.</t>
     </r>
   </si>
   <si>
@@ -1486,7 +1499,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Tekniker</t>
+      <t>Tekniker</t>
     </r>
     <r>
       <rPr>
@@ -1495,7 +1508,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">is an independent research organization, whose main working focus is to improve manufacturing technologies, that includes all the situations that characterises a product life cycle, from conception and design, until the end of working life. Automotive parts, machine tools, mechanical capital goods, aerospace, chemical and petroleum products and industrial and consumer electronics are the most relevant sectors served by Tekniker.Tekniker likes to define itself as a Mechatronics, Manufacturing Technologies and Microtechnologies centre. It mainly specialises in: designing consumer and industrial products, solving problems relating to friction, wear and lubrication, incorporating information technologies and communications in the plant, high precision, miniaturisation and micro/nanotechnologies.</t>
+      <t>is an independent research organization, whose main working focus is to improve manufacturing technologies, that includes all the situations that characterises a product life cycle, from conception and design, until the end of working life. Automotive parts, machine tools, mechanical capital goods, aerospace, chemical and petroleum products and industrial and consumer electronics are the most relevant sectors served by Tekniker.Tekniker likes to define itself as a Mechatronics, Manufacturing Technologies and Microtechnologies centre. It mainly specialises in: designing consumer and industrial products, solving problems relating to friction, wear and lubrication, incorporating information technologies and communications in the plant, high precision, miniaturisation and micro/nanotechnologies.</t>
     </r>
   </si>
   <si>
@@ -1508,6 +1521,24 @@
     <t>https://www.secpho.org/wp-content/uploads/2013/10/logo-tekniker-ajustado-okok-250x100.jpg</t>
   </si>
   <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Descuento</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>user4</t>
+  </si>
+  <si>
     <t>Tipos de empresas</t>
   </si>
   <si>
@@ -1725,225 +1756,12 @@
   </si>
   <si>
     <t>Administración pública</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>8eUBY7AUET_P</t>
-  </si>
-  <si>
-    <t>z8nsyh^&gt;lxpI</t>
-  </si>
-  <si>
-    <t>eVJ7fTNqr3bW</t>
-  </si>
-  <si>
-    <t>_[OSGev30mXI</t>
-  </si>
-  <si>
-    <t>=a=nt5oEejw3</t>
-  </si>
-  <si>
-    <t>S^5Xz;qIalfr</t>
-  </si>
-  <si>
-    <t>PoL=oxEvOGxi</t>
-  </si>
-  <si>
-    <t>WV3ymqMoi[?h</t>
-  </si>
-  <si>
-    <t>d\xZVLj:^_&gt;K</t>
-  </si>
-  <si>
-    <t>D0ZksFRpa@l9</t>
-  </si>
-  <si>
-    <t>X;C&lt;IoEa5@3D</t>
-  </si>
-  <si>
-    <t>YWu`tQDyaXKs</t>
-  </si>
-  <si>
-    <t>oO3pxk?jJaH9</t>
-  </si>
-  <si>
-    <t>1ep&lt;Aw&gt;UPStq</t>
-  </si>
-  <si>
-    <t>Ab=vWYMK&gt;0^m</t>
-  </si>
-  <si>
-    <t>8mzm^YK@MD0V</t>
-  </si>
-  <si>
-    <t>95^VAx[AS49b</t>
-  </si>
-  <si>
-    <t>&gt;49CoLxMd]bK</t>
-  </si>
-  <si>
-    <t>b4Z\;KFifGmH</t>
-  </si>
-  <si>
-    <t>\c5E@hvu2m\h</t>
-  </si>
-  <si>
-    <t>cN&gt;dD=FFXwt2</t>
-  </si>
-  <si>
-    <t>W_@4eZLDJ?&lt;]</t>
-  </si>
-  <si>
-    <t>H46EwKK1S1FZ</t>
-  </si>
-  <si>
-    <t>0KZg\=sj4PgX</t>
-  </si>
-  <si>
-    <t>no7Ly_d`?Uyb</t>
-  </si>
-  <si>
-    <t>IwyFoXkzYgvm</t>
-  </si>
-  <si>
-    <t>_20Np2RUeht@</t>
-  </si>
-  <si>
-    <t>6y_:E3=`qiG`</t>
-  </si>
-  <si>
-    <t>H_&lt;zbiPX[0oH</t>
-  </si>
-  <si>
-    <t>HNv6qmr`l;uX</t>
-  </si>
-  <si>
-    <t>xqH@dV1\N3xi</t>
-  </si>
-  <si>
-    <t>qX\3Ev?KF&gt;tj</t>
-  </si>
-  <si>
-    <t>bE=Mr_5c[NKq</t>
-  </si>
-  <si>
-    <t>JsL&lt;Ly4&lt;wB4\</t>
-  </si>
-  <si>
-    <t>Pv&gt;a45@]MADL</t>
-  </si>
-  <si>
-    <t>2hM;?ISngPXq</t>
-  </si>
-  <si>
-    <t>akMUsG\MfEmG</t>
-  </si>
-  <si>
-    <t>6?7?LO\Qoc]k</t>
-  </si>
-  <si>
-    <t>wlccB=72FO6e</t>
-  </si>
-  <si>
-    <t>K[1e^kL^]nOe</t>
-  </si>
-  <si>
-    <t>fXqZyJC=lxKZ</t>
-  </si>
-  <si>
-    <t>YF81V[Q=M6]g</t>
-  </si>
-  <si>
-    <t>X&gt;F[5et`Km9\</t>
-  </si>
-  <si>
-    <t>eXXH[S=GxIi&lt;</t>
-  </si>
-  <si>
-    <t>5fmnK7MeuvDR</t>
-  </si>
-  <si>
-    <t>&gt;YoMIZ6ZWZ8k</t>
-  </si>
-  <si>
-    <t>F7dwv1_7;FuF</t>
-  </si>
-  <si>
-    <t>0Mw8xE2QPm5T</t>
-  </si>
-  <si>
-    <t>W_=HLj\aO:cM</t>
-  </si>
-  <si>
-    <t>Qfu9M&gt;MPRjXA</t>
-  </si>
-  <si>
-    <t>n@F7DgDE_oXC</t>
-  </si>
-  <si>
-    <t>rA3\`tForLUq</t>
-  </si>
-  <si>
-    <t>UYBtTR@Z[eMC</t>
-  </si>
-  <si>
-    <t>vH[TM]e1bdDf</t>
-  </si>
-  <si>
-    <t>Z3`96uyn7fQc</t>
-  </si>
-  <si>
-    <t>6jRL:6QcpCzY</t>
-  </si>
-  <si>
-    <t>EEHz1hanRiq]</t>
-  </si>
-  <si>
-    <t>?8X^hN:XUggA</t>
-  </si>
-  <si>
-    <t>OwcU2Dw;jsA6</t>
-  </si>
-  <si>
-    <t>UtGui3\DnG=i</t>
-  </si>
-  <si>
-    <t>tYoRi3lU?DnB</t>
-  </si>
-  <si>
-    <t>]XimGJEbCD12</t>
-  </si>
-  <si>
-    <t>^_DLrsEztL29</t>
-  </si>
-  <si>
-    <t>zJ=r=DY9ECD@</t>
-  </si>
-  <si>
-    <t>?6ef]j?DGHku</t>
-  </si>
-  <si>
-    <t>0i&gt;uqNIlpoEq</t>
-  </si>
-  <si>
-    <t>wI`vJPz5Zob_</t>
-  </si>
-  <si>
-    <t>K=vXh:;VohcJ</t>
-  </si>
-  <si>
-    <t>&lt;YfDHoww4C7s</t>
-  </si>
-  <si>
-    <t>;[58ZUYWqni4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -2137,45 +1955,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFill="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFill="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="2" applyFill="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="2" applyFill="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyFill="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFill="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFill="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFill="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2185,7 +2003,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFill="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2209,25 +2027,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
-      <protection locked="0" hidden="0"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
+    <cellStyle name="Bueno" xfId="3" builtinId="26"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Incorrecto" xfId="6" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Hyperlink" xfId="1"/>
     <cellStyle name="Salida" xfId="2" builtinId="21"/>
-    <cellStyle name="Bueno" xfId="3" builtinId="26"/>
-    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
-    <cellStyle name="Hipervínculo" xfId="5" builtinId="8"/>
-    <cellStyle name="Incorrecto" xfId="6" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2495,14 +2319,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14062" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
@@ -2584,9 +2408,6 @@
       <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" t="s">
-        <v>534</v>
-      </c>
     </row>
     <row r="3" spans="1:11" ht="30">
       <c r="A3" s="13" t="s">
@@ -2619,9 +2440,6 @@
       <c r="J3" t="s">
         <v>23</v>
       </c>
-      <c r="K3" t="s">
-        <v>535</v>
-      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="13" t="s">
@@ -2654,9 +2472,6 @@
       <c r="J4" t="s">
         <v>27</v>
       </c>
-      <c r="K4" t="s">
-        <v>536</v>
-      </c>
     </row>
     <row r="5" spans="1:11" ht="45">
       <c r="A5" s="13" t="s">
@@ -2689,9 +2504,6 @@
       <c r="J5" t="s">
         <v>31</v>
       </c>
-      <c r="K5" t="s">
-        <v>537</v>
-      </c>
     </row>
     <row r="6" spans="1:11" ht="30">
       <c r="A6" s="13" t="s">
@@ -2724,9 +2536,6 @@
       <c r="J6" t="s">
         <v>35</v>
       </c>
-      <c r="K6" t="s">
-        <v>538</v>
-      </c>
     </row>
     <row r="7" spans="1:11" ht="45">
       <c r="A7" s="13" t="s">
@@ -2759,9 +2568,6 @@
       <c r="J7" t="s">
         <v>43</v>
       </c>
-      <c r="K7" t="s">
-        <v>539</v>
-      </c>
     </row>
     <row r="8" spans="1:11" ht="45">
       <c r="A8" s="13" t="s">
@@ -2794,9 +2600,6 @@
       <c r="J8" t="s">
         <v>47</v>
       </c>
-      <c r="K8" t="s">
-        <v>540</v>
-      </c>
     </row>
     <row r="9" spans="1:11" ht="30">
       <c r="A9" s="13" t="s">
@@ -2829,9 +2632,6 @@
       <c r="J9" t="s">
         <v>51</v>
       </c>
-      <c r="K9" t="s">
-        <v>541</v>
-      </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="13" t="s">
@@ -2864,9 +2664,6 @@
       <c r="J10" t="s">
         <v>56</v>
       </c>
-      <c r="K10" t="s">
-        <v>542</v>
-      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="13" t="s">
@@ -2899,9 +2696,6 @@
       <c r="J11" t="s">
         <v>60</v>
       </c>
-      <c r="K11" t="s">
-        <v>543</v>
-      </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="13" t="s">
@@ -2934,9 +2728,6 @@
       <c r="J12" t="s">
         <v>68</v>
       </c>
-      <c r="K12" t="s">
-        <v>544</v>
-      </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="13" t="s">
@@ -2969,9 +2760,6 @@
       <c r="J13" t="s">
         <v>72</v>
       </c>
-      <c r="K13" t="s">
-        <v>545</v>
-      </c>
     </row>
     <row r="14" spans="1:11" ht="60">
       <c r="A14" s="13" t="s">
@@ -3003,9 +2791,6 @@
       </c>
       <c r="J14" t="s">
         <v>76</v>
-      </c>
-      <c r="K14" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="90">
@@ -3033,9 +2818,6 @@
       <c r="J15" t="s">
         <v>81</v>
       </c>
-      <c r="K15" t="s">
-        <v>547</v>
-      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="13" t="s">
@@ -3062,11 +2844,8 @@
       <c r="J16" t="s">
         <v>85</v>
       </c>
-      <c r="K16" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="75">
+    </row>
+    <row r="17" spans="1:10" ht="75">
       <c r="A17" s="13" t="s">
         <v>86</v>
       </c>
@@ -3091,11 +2870,8 @@
       <c r="J17" t="s">
         <v>89</v>
       </c>
-      <c r="K17" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="45">
+    </row>
+    <row r="18" spans="1:10" ht="45">
       <c r="A18" s="13" t="s">
         <v>90</v>
       </c>
@@ -3120,11 +2896,8 @@
       <c r="J18" t="s">
         <v>93</v>
       </c>
-      <c r="K18" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="60">
+    </row>
+    <row r="19" spans="1:10" ht="60">
       <c r="A19" s="13" t="s">
         <v>94</v>
       </c>
@@ -3149,11 +2922,8 @@
       <c r="J19" t="s">
         <v>97</v>
       </c>
-      <c r="K19" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="45">
+    </row>
+    <row r="20" spans="1:10" ht="45">
       <c r="A20" s="13" t="s">
         <v>98</v>
       </c>
@@ -3178,11 +2948,8 @@
       <c r="J20" t="s">
         <v>101</v>
       </c>
-      <c r="K20" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="30">
+    </row>
+    <row r="21" spans="1:10" ht="30">
       <c r="A21" s="13" t="s">
         <v>102</v>
       </c>
@@ -3207,11 +2974,8 @@
       <c r="J21" t="s">
         <v>105</v>
       </c>
-      <c r="K21" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="30">
+    </row>
+    <row r="22" spans="1:10" ht="30">
       <c r="A22" s="13" t="s">
         <v>106</v>
       </c>
@@ -3236,11 +3000,8 @@
       <c r="J22" t="s">
         <v>109</v>
       </c>
-      <c r="K22" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" s="13" t="s">
         <v>110</v>
       </c>
@@ -3265,11 +3026,8 @@
       <c r="J23" t="s">
         <v>113</v>
       </c>
-      <c r="K23" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="30">
+    </row>
+    <row r="24" spans="1:10" ht="30">
       <c r="A24" s="13" t="s">
         <v>114</v>
       </c>
@@ -3294,11 +3052,8 @@
       <c r="J24" t="s">
         <v>117</v>
       </c>
-      <c r="K24" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="45">
+    </row>
+    <row r="25" spans="1:10" ht="45">
       <c r="A25" s="13" t="s">
         <v>118</v>
       </c>
@@ -3323,11 +3078,8 @@
       <c r="J25" t="s">
         <v>122</v>
       </c>
-      <c r="K25" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="30">
+    </row>
+    <row r="26" spans="1:10" ht="30">
       <c r="A26" s="13" t="s">
         <v>123</v>
       </c>
@@ -3352,11 +3104,8 @@
       <c r="J26" t="s">
         <v>126</v>
       </c>
-      <c r="K26" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="30">
+    </row>
+    <row r="27" spans="1:10" ht="30">
       <c r="A27" s="13" t="s">
         <v>127</v>
       </c>
@@ -3381,11 +3130,8 @@
       <c r="J27" t="s">
         <v>130</v>
       </c>
-      <c r="K27" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="30">
+    </row>
+    <row r="28" spans="1:10" ht="30">
       <c r="A28" s="13" t="s">
         <v>131</v>
       </c>
@@ -3410,11 +3156,8 @@
       <c r="J28" t="s">
         <v>134</v>
       </c>
-      <c r="K28" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="30">
+    </row>
+    <row r="29" spans="1:10" ht="30">
       <c r="A29" s="13" t="s">
         <v>135</v>
       </c>
@@ -3439,11 +3182,8 @@
       <c r="J29" t="s">
         <v>138</v>
       </c>
-      <c r="K29" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="30">
+    </row>
+    <row r="30" spans="1:10" ht="30">
       <c r="A30" s="13" t="s">
         <v>139</v>
       </c>
@@ -3468,11 +3208,8 @@
       <c r="J30" t="s">
         <v>142</v>
       </c>
-      <c r="K30" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" s="13" t="s">
         <v>143</v>
       </c>
@@ -3497,11 +3234,8 @@
       <c r="J31" t="s">
         <v>146</v>
       </c>
-      <c r="K31" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="45">
+    </row>
+    <row r="32" spans="1:10" ht="45">
       <c r="A32" s="13" t="s">
         <v>147</v>
       </c>
@@ -3526,11 +3260,8 @@
       <c r="J32" t="s">
         <v>151</v>
       </c>
-      <c r="K32" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="45">
+    </row>
+    <row r="33" spans="1:10" ht="45">
       <c r="A33" s="13" t="s">
         <v>152</v>
       </c>
@@ -3555,11 +3286,8 @@
       <c r="J33" t="s">
         <v>155</v>
       </c>
-      <c r="K33" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="30">
+    </row>
+    <row r="34" spans="1:10" ht="30">
       <c r="A34" s="13" t="s">
         <v>156</v>
       </c>
@@ -3590,11 +3318,8 @@
       <c r="J34" t="s">
         <v>163</v>
       </c>
-      <c r="K34" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="30">
+    </row>
+    <row r="35" spans="1:10" ht="30">
       <c r="A35" s="13" t="s">
         <v>164</v>
       </c>
@@ -3625,11 +3350,8 @@
       <c r="J35" t="s">
         <v>167</v>
       </c>
-      <c r="K35" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="30">
+    </row>
+    <row r="36" spans="1:10" ht="30">
       <c r="A36" s="13" t="s">
         <v>168</v>
       </c>
@@ -3654,11 +3376,8 @@
       <c r="J36" t="s">
         <v>171</v>
       </c>
-      <c r="K36" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="30">
+    </row>
+    <row r="37" spans="1:10" ht="30">
       <c r="A37" s="13" t="s">
         <v>172</v>
       </c>
@@ -3683,11 +3402,8 @@
       <c r="J37" t="s">
         <v>175</v>
       </c>
-      <c r="K37" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="30">
+    </row>
+    <row r="38" spans="1:10" ht="30">
       <c r="A38" s="13" t="s">
         <v>176</v>
       </c>
@@ -3712,11 +3428,8 @@
       <c r="J38" t="s">
         <v>180</v>
       </c>
-      <c r="K38" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="30">
+    </row>
+    <row r="39" spans="1:10" ht="30">
       <c r="A39" s="13" t="s">
         <v>181</v>
       </c>
@@ -3741,11 +3454,8 @@
       <c r="J39" t="s">
         <v>184</v>
       </c>
-      <c r="K39" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40" s="13" t="s">
         <v>185</v>
       </c>
@@ -3770,11 +3480,8 @@
       <c r="J40" t="s">
         <v>188</v>
       </c>
-      <c r="K40" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41" s="13" t="s">
         <v>189</v>
       </c>
@@ -3799,11 +3506,8 @@
       <c r="J41" t="s">
         <v>192</v>
       </c>
-      <c r="K41" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="30">
+    </row>
+    <row r="42" spans="1:10" ht="30">
       <c r="A42" s="13" t="s">
         <v>193</v>
       </c>
@@ -3828,11 +3532,8 @@
       <c r="J42" t="s">
         <v>196</v>
       </c>
-      <c r="K42" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" ht="30">
+    </row>
+    <row r="43" spans="1:10" ht="30">
       <c r="A43" s="13" t="s">
         <v>197</v>
       </c>
@@ -3857,11 +3558,8 @@
       <c r="J43" t="s">
         <v>200</v>
       </c>
-      <c r="K43" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11">
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44" s="13" t="s">
         <v>201</v>
       </c>
@@ -3892,11 +3590,8 @@
       <c r="J44" t="s">
         <v>208</v>
       </c>
-      <c r="K44" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11">
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45" s="13" t="s">
         <v>209</v>
       </c>
@@ -3927,11 +3622,8 @@
       <c r="J45" t="s">
         <v>212</v>
       </c>
-      <c r="K45" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" ht="30">
+    </row>
+    <row r="46" spans="1:10" ht="30">
       <c r="A46" s="13" t="s">
         <v>213</v>
       </c>
@@ -3962,11 +3654,8 @@
       <c r="J46" t="s">
         <v>215</v>
       </c>
-      <c r="K46" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="30">
+    </row>
+    <row r="47" spans="1:10" ht="30">
       <c r="A47" s="13" t="s">
         <v>216</v>
       </c>
@@ -3997,11 +3686,8 @@
       <c r="J47" t="s">
         <v>222</v>
       </c>
-      <c r="K47" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" ht="30">
+    </row>
+    <row r="48" spans="1:10" ht="30">
       <c r="A48" s="13" t="s">
         <v>223</v>
       </c>
@@ -4032,11 +3718,8 @@
       <c r="J48" t="s">
         <v>226</v>
       </c>
-      <c r="K48" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11">
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49" s="13" t="s">
         <v>227</v>
       </c>
@@ -4067,11 +3750,8 @@
       <c r="J49" t="s">
         <v>234</v>
       </c>
-      <c r="K49" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" ht="60">
+    </row>
+    <row r="50" spans="1:10" ht="60">
       <c r="A50" s="13" t="s">
         <v>235</v>
       </c>
@@ -4102,11 +3782,8 @@
       <c r="J50" t="s">
         <v>239</v>
       </c>
-      <c r="K50" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="60">
+    </row>
+    <row r="51" spans="1:10" ht="60">
       <c r="A51" s="13" t="s">
         <v>240</v>
       </c>
@@ -4137,11 +3814,8 @@
       <c r="J51" t="s">
         <v>247</v>
       </c>
-      <c r="K51" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="60">
+    </row>
+    <row r="52" spans="1:10" ht="60">
       <c r="A52" s="13" t="s">
         <v>248</v>
       </c>
@@ -4172,11 +3846,8 @@
       <c r="J52" t="s">
         <v>251</v>
       </c>
-      <c r="K52" t="s">
-        <v>584</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" ht="105">
+    </row>
+    <row r="53" spans="1:10" ht="105">
       <c r="A53" s="13" t="s">
         <v>252</v>
       </c>
@@ -4207,11 +3878,8 @@
       <c r="J53" t="s">
         <v>259</v>
       </c>
-      <c r="K53" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" ht="30">
+    </row>
+    <row r="54" spans="1:10" ht="30">
       <c r="A54" s="13" t="s">
         <v>260</v>
       </c>
@@ -4242,11 +3910,8 @@
       <c r="J54" t="s">
         <v>267</v>
       </c>
-      <c r="K54" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="30">
+    </row>
+    <row r="55" spans="1:10" ht="30">
       <c r="A55" s="13" t="s">
         <v>268</v>
       </c>
@@ -4277,11 +3942,8 @@
       <c r="J55" t="s">
         <v>271</v>
       </c>
-      <c r="K55" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="26.25">
+    </row>
+    <row r="56" spans="1:10" ht="26.25">
       <c r="A56" s="13" t="s">
         <v>272</v>
       </c>
@@ -4312,11 +3974,8 @@
       <c r="J56" t="s">
         <v>274</v>
       </c>
-      <c r="K56" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" ht="30">
+    </row>
+    <row r="57" spans="1:10" ht="30">
       <c r="A57" s="13" t="s">
         <v>275</v>
       </c>
@@ -4347,11 +4006,8 @@
       <c r="J57" t="s">
         <v>280</v>
       </c>
-      <c r="K57" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11">
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58" s="13" t="s">
         <v>281</v>
       </c>
@@ -4382,11 +4038,8 @@
       <c r="J58" t="s">
         <v>284</v>
       </c>
-      <c r="K58" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="30">
+    </row>
+    <row r="59" spans="1:10" ht="30">
       <c r="A59" s="13" t="s">
         <v>285</v>
       </c>
@@ -4417,11 +4070,8 @@
       <c r="J59" t="s">
         <v>288</v>
       </c>
-      <c r="K59" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11">
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60" s="13" t="s">
         <v>289</v>
       </c>
@@ -4452,11 +4102,8 @@
       <c r="J60" t="s">
         <v>292</v>
       </c>
-      <c r="K60" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11">
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61" s="13" t="s">
         <v>293</v>
       </c>
@@ -4487,11 +4134,8 @@
       <c r="J61" t="s">
         <v>300</v>
       </c>
-      <c r="K61" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="60">
+    </row>
+    <row r="62" spans="1:10" ht="60">
       <c r="A62" s="13" t="s">
         <v>301</v>
       </c>
@@ -4522,11 +4166,8 @@
       <c r="J62" t="s">
         <v>307</v>
       </c>
-      <c r="K62" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="45">
+    </row>
+    <row r="63" spans="1:10" ht="45">
       <c r="A63" s="13" t="s">
         <v>308</v>
       </c>
@@ -4557,11 +4198,8 @@
       <c r="J63" t="s">
         <v>311</v>
       </c>
-      <c r="K63" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11">
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64" s="13" t="s">
         <v>312</v>
       </c>
@@ -4592,11 +4230,8 @@
       <c r="J64" t="s">
         <v>314</v>
       </c>
-      <c r="K64" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11">
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65" s="13" t="s">
         <v>315</v>
       </c>
@@ -4627,11 +4262,8 @@
       <c r="J65" t="s">
         <v>318</v>
       </c>
-      <c r="K65" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" ht="45">
+    </row>
+    <row r="66" spans="1:10" ht="45">
       <c r="A66" s="13" t="s">
         <v>319</v>
       </c>
@@ -4662,11 +4294,8 @@
       <c r="J66" t="s">
         <v>322</v>
       </c>
-      <c r="K66" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" ht="30">
+    </row>
+    <row r="67" spans="1:10" ht="30">
       <c r="A67" s="13" t="s">
         <v>323</v>
       </c>
@@ -4697,11 +4326,8 @@
       <c r="J67" t="s">
         <v>329</v>
       </c>
-      <c r="K67" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="30">
+    </row>
+    <row r="68" spans="1:10" ht="30">
       <c r="A68" s="13" t="s">
         <v>330</v>
       </c>
@@ -4732,11 +4358,8 @@
       <c r="J68" t="s">
         <v>336</v>
       </c>
-      <c r="K68" t="s">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="30">
+    </row>
+    <row r="69" spans="1:10" ht="30">
       <c r="A69" s="13" t="s">
         <v>337</v>
       </c>
@@ -4767,11 +4390,8 @@
       <c r="J69" t="s">
         <v>340</v>
       </c>
-      <c r="K69" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11">
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70" s="13" t="s">
         <v>341</v>
       </c>
@@ -4796,11 +4416,8 @@
       <c r="J70" t="s">
         <v>344</v>
       </c>
-      <c r="K70" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" ht="45">
+    </row>
+    <row r="71" spans="1:10" ht="45">
       <c r="A71" s="13" t="s">
         <v>345</v>
       </c>
@@ -4830,44 +4447,41 @@
       </c>
       <c r="J71" t="s">
         <v>350</v>
-      </c>
-      <c r="K71" t="s">
-        <v>603</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
   <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <g2:dataValidations xmlns:g2="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" count="2">
-        <g2:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
-          <g2:formula1>
-            <g3:f xmlns:g3="http://schemas.microsoft.com/office/excel/2006/main">'Listas y leyendas'!$F$2:$F$9</g3:f>
-          </g2:formula1>
-          <g3:sqref xmlns:g3="http://schemas.microsoft.com/office/excel/2006/main">E72:E1048576</g3:sqref>
-        </g2:dataValidation>
-        <g2:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
-          <g2:formula1>
-            <g3:f xmlns:g3="http://schemas.microsoft.com/office/excel/2006/main">'Listas y leyendas'!$O$2:$O$10</g3:f>
-          </g2:formula1>
-          <g3:sqref xmlns:g3="http://schemas.microsoft.com/office/excel/2006/main">H72:H1048576</g3:sqref>
-        </g2:dataValidation>
-      </g2:dataValidations>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+          <x14:formula1>
+            <xm:f>'Listas y leyendas'!$F$2:$F$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>E72:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
+          <x14:formula1>
+            <xm:f>'Listas y leyendas'!$O$2:$O$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>H72:H1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14062" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.85546875" customWidth="1"/>
     <col min="2" max="2" width="76.5703125" customWidth="1"/>
@@ -4935,9 +4549,6 @@
       <c r="H2" t="s">
         <v>364</v>
       </c>
-      <c r="I2" t="s">
-        <v>533</v>
-      </c>
     </row>
     <row r="3" spans="1:9" ht="195">
       <c r="A3" t="s">
@@ -4964,9 +4575,6 @@
       <c r="H3" t="s">
         <v>368</v>
       </c>
-      <c r="I3" t="s">
-        <v>533</v>
-      </c>
     </row>
     <row r="4" spans="1:9" ht="180">
       <c r="A4" t="s">
@@ -4993,9 +4601,6 @@
       <c r="H4" t="s">
         <v>372</v>
       </c>
-      <c r="I4" t="s">
-        <v>533</v>
-      </c>
     </row>
     <row r="5" spans="1:9" ht="270">
       <c r="A5" t="s">
@@ -5022,9 +4627,6 @@
       <c r="H5" t="s">
         <v>376</v>
       </c>
-      <c r="I5" t="s">
-        <v>533</v>
-      </c>
     </row>
     <row r="6" spans="1:9" ht="165">
       <c r="A6" t="s">
@@ -5051,9 +4653,6 @@
       <c r="H6" t="s">
         <v>380</v>
       </c>
-      <c r="I6" t="s">
-        <v>533</v>
-      </c>
     </row>
     <row r="7" spans="1:9" ht="120">
       <c r="A7" t="s">
@@ -5080,9 +4679,6 @@
       <c r="H7" t="s">
         <v>384</v>
       </c>
-      <c r="I7" t="s">
-        <v>533</v>
-      </c>
     </row>
     <row r="8" spans="1:9" ht="51.75">
       <c r="A8" t="s">
@@ -5109,9 +4705,6 @@
       <c r="H8" t="s">
         <v>388</v>
       </c>
-      <c r="I8" t="s">
-        <v>533</v>
-      </c>
     </row>
     <row r="9" spans="1:9" ht="102.75">
       <c r="A9" t="s">
@@ -5138,9 +4731,6 @@
       <c r="H9" t="s">
         <v>392</v>
       </c>
-      <c r="I9" t="s">
-        <v>533</v>
-      </c>
     </row>
     <row r="10" spans="1:9" ht="315">
       <c r="A10" t="s">
@@ -5167,9 +4757,6 @@
       <c r="H10" t="s">
         <v>396</v>
       </c>
-      <c r="I10" t="s">
-        <v>533</v>
-      </c>
     </row>
     <row r="11" spans="1:9" ht="405">
       <c r="A11" t="s">
@@ -5196,9 +4783,6 @@
       <c r="H11" t="s">
         <v>400</v>
       </c>
-      <c r="I11" t="s">
-        <v>533</v>
-      </c>
     </row>
     <row r="12" spans="1:9" ht="90">
       <c r="A12" t="s">
@@ -5225,9 +4809,6 @@
       <c r="H12" t="s">
         <v>404</v>
       </c>
-      <c r="I12" t="s">
-        <v>533</v>
-      </c>
     </row>
     <row r="13" spans="1:9" ht="102.75">
       <c r="A13" t="s">
@@ -5254,9 +4835,6 @@
       <c r="H13" t="s">
         <v>408</v>
       </c>
-      <c r="I13" t="s">
-        <v>533</v>
-      </c>
     </row>
     <row r="14" spans="1:9" ht="345">
       <c r="A14" t="s">
@@ -5283,9 +4861,6 @@
       <c r="H14" t="s">
         <v>412</v>
       </c>
-      <c r="I14" t="s">
-        <v>533</v>
-      </c>
     </row>
     <row r="15" spans="1:9" ht="150">
       <c r="A15" t="s">
@@ -5312,9 +4887,6 @@
       <c r="H15" t="s">
         <v>416</v>
       </c>
-      <c r="I15" t="s">
-        <v>533</v>
-      </c>
     </row>
     <row r="16" spans="1:9" ht="77.25">
       <c r="A16" t="s">
@@ -5341,11 +4913,8 @@
       <c r="H16" t="s">
         <v>420</v>
       </c>
-      <c r="I16" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="75">
+    </row>
+    <row r="17" spans="1:8" ht="75">
       <c r="A17" t="s">
         <v>242</v>
       </c>
@@ -5370,11 +4939,8 @@
       <c r="H17" t="s">
         <v>424</v>
       </c>
-      <c r="I17" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="375">
+    </row>
+    <row r="18" spans="1:8" ht="375">
       <c r="A18" t="s">
         <v>254</v>
       </c>
@@ -5399,11 +4965,8 @@
       <c r="H18" t="s">
         <v>428</v>
       </c>
-      <c r="I18" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="102.75">
+    </row>
+    <row r="19" spans="1:8" ht="102.75">
       <c r="A19" t="s">
         <v>262</v>
       </c>
@@ -5428,11 +4991,8 @@
       <c r="H19" t="s">
         <v>432</v>
       </c>
-      <c r="I19" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="51" customHeight="1">
+    </row>
+    <row r="20" spans="1:8" ht="51" customHeight="1">
       <c r="A20" t="s">
         <v>277</v>
       </c>
@@ -5457,11 +5017,8 @@
       <c r="H20" t="s">
         <v>436</v>
       </c>
-      <c r="I20" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="115.5">
+    </row>
+    <row r="21" spans="1:8" ht="115.5">
       <c r="A21" t="s">
         <v>295</v>
       </c>
@@ -5486,11 +5043,8 @@
       <c r="H21" t="s">
         <v>440</v>
       </c>
-      <c r="I21" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="102.75">
+    </row>
+    <row r="22" spans="1:8" ht="102.75">
       <c r="A22" t="s">
         <v>303</v>
       </c>
@@ -5515,11 +5069,8 @@
       <c r="H22" t="s">
         <v>444</v>
       </c>
-      <c r="I22" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="115.5">
+    </row>
+    <row r="23" spans="1:8" ht="115.5">
       <c r="A23" t="s">
         <v>324</v>
       </c>
@@ -5544,11 +5095,8 @@
       <c r="H23" t="s">
         <v>448</v>
       </c>
-      <c r="I23" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="64.5">
+    </row>
+    <row r="24" spans="1:8" ht="64.5">
       <c r="A24" t="s">
         <v>338</v>
       </c>
@@ -5573,11 +5121,8 @@
       <c r="H24" t="s">
         <v>452</v>
       </c>
-      <c r="I24" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="38.25">
+    </row>
+    <row r="25" spans="1:8" ht="38.25">
       <c r="A25" t="s">
         <v>342</v>
       </c>
@@ -5602,11 +5147,8 @@
       <c r="H25" t="s">
         <v>455</v>
       </c>
-      <c r="I25" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="128.25">
+    </row>
+    <row r="26" spans="1:8" ht="128.25">
       <c r="A26" t="s">
         <v>347</v>
       </c>
@@ -5631,57 +5173,113 @@
       <c r="H26" t="s">
         <v>459</v>
       </c>
-      <c r="I26" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+    </row>
+    <row r="27" spans="1:8">
       <c r="B27" s="20"/>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:8">
       <c r="B28" s="21"/>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:8">
       <c r="B29" s="21"/>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:8">
       <c r="B30" s="20"/>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:8">
       <c r="B31" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
-    <ext uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <g2:dataValidations xmlns:g2="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" count="2">
-        <g2:dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" type="list">
-          <g2:formula1>
-            <g3:f xmlns:g3="http://schemas.microsoft.com/office/excel/2006/main">'Listas y leyendas'!$F$2:$F$9</g3:f>
-          </g2:formula1>
-          <g3:sqref xmlns:g3="http://schemas.microsoft.com/office/excel/2006/main">A2</g3:sqref>
-        </g2:dataValidation>
-        <g2:dataValidation allowBlank="1" error="Seleccione un valor de la lista" errorTitle="Entrada inválida" prompt="Seleccione un tipo de empresa" promptTitle="Tipo de empresa" showErrorMessage="1" showInputMessage="1" type="list">
-          <g2:formula1>
-            <g3:f xmlns:g3="http://schemas.microsoft.com/office/excel/2006/main">'Listas y leyendas'!$B$2:$B$21</g3:f>
-          </g2:formula1>
-          <g3:sqref xmlns:g3="http://schemas.microsoft.com/office/excel/2006/main">D2:D1048576</g3:sqref>
-        </g2:dataValidation>
-      </g2:dataValidations>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
+          <x14:formula1>
+            <xm:f>'Listas y leyendas'!$F$2:$F$9</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Entrada inválida" error="Seleccione un valor de la lista" promptTitle="Tipo de empresa" prompt="Seleccione un tipo de empresa" xr:uid="{00000000-0002-0000-0100-000001000000}">
+          <x14:formula1>
+            <xm:f>'Listas y leyendas'!$B$2:$B$21</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C876676D-DD75-4785-895D-73121CF7C510}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19" style="8" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="32" t="s">
+        <v>460</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="B2" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="8" t="s">
+        <v>463</v>
+      </c>
+      <c r="B3" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="B4" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="B5" s="9">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14062" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="39.5703125" customWidth="1"/>
     <col min="5" max="5" width="30.85546875" customWidth="1"/>
@@ -5692,43 +5290,43 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75">
       <c r="A1" s="3" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="5" t="s">
-        <v>462</v>
+        <v>468</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="6" t="s">
-        <v>463</v>
+        <v>469</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="J1" s="4"/>
       <c r="K1" s="7" t="s">
-        <v>464</v>
+        <v>470</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75">
       <c r="A2" s="2" t="s">
-        <v>465</v>
+        <v>471</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -5736,27 +5334,27 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="2" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="2" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="I2" s="2">
         <v>0</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="2" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
       <c r="L2" s="2">
         <v>0</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="O2" s="2">
         <v>0</v>
@@ -5764,7 +5362,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75">
       <c r="A3" s="2" t="s">
-        <v>470</v>
+        <v>476</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -5772,27 +5370,27 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="2" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="2" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="I3" s="2">
         <v>1</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="2" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="L3" s="2">
         <v>1</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="O3" s="2">
         <v>1</v>
@@ -5800,7 +5398,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.75">
       <c r="A4" s="2" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -5808,27 +5406,27 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="2" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="F4" s="2">
         <v>2</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="2" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="I4" s="2">
         <v>2</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="2" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="L4" s="2">
         <v>2</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="O4" s="2">
         <v>2</v>
@@ -5836,7 +5434,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75">
       <c r="A5" s="2" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
@@ -5844,27 +5442,27 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="2" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="F5" s="2">
         <v>3</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="2" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
       <c r="I5" s="2">
         <v>3</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="2" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="L5" s="2">
         <v>3</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
       <c r="O5" s="2">
         <v>3</v>
@@ -5872,7 +5470,7 @@
     </row>
     <row r="6" spans="1:15" ht="15.75">
       <c r="A6" s="2" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
@@ -5880,27 +5478,27 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="2" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
       <c r="F6" s="2">
         <v>4</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="2" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="I6" s="2">
         <v>4</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="2" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
       <c r="L6" s="2">
         <v>4</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
       <c r="O6" s="2">
         <v>4</v>
@@ -5908,7 +5506,7 @@
     </row>
     <row r="7" spans="1:15" ht="15.75">
       <c r="A7" s="2" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
@@ -5916,27 +5514,27 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="2" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="F7" s="2">
         <v>5</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="2" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
       <c r="I7" s="2">
         <v>5</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="2" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="L7" s="2">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>494</v>
+        <v>500</v>
       </c>
       <c r="O7" s="2">
         <v>5</v>
@@ -5944,7 +5542,7 @@
     </row>
     <row r="8" spans="1:15" ht="15.75">
       <c r="A8" s="2" t="s">
-        <v>495</v>
+        <v>501</v>
       </c>
       <c r="B8" s="2">
         <v>6</v>
@@ -5952,27 +5550,27 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="2" t="s">
-        <v>496</v>
+        <v>502</v>
       </c>
       <c r="F8" s="2">
         <v>6</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="2" t="s">
-        <v>497</v>
+        <v>503</v>
       </c>
       <c r="I8" s="2">
         <v>6</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="2" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c r="L8" s="2">
         <v>6</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="O8" s="2">
         <v>6</v>
@@ -5980,7 +5578,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75">
       <c r="A9" s="2" t="s">
-        <v>500</v>
+        <v>506</v>
       </c>
       <c r="B9" s="2">
         <v>7</v>
@@ -5988,27 +5586,27 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="2" t="s">
-        <v>501</v>
+        <v>507</v>
       </c>
       <c r="F9" s="2">
         <v>7</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="2" t="s">
-        <v>502</v>
+        <v>508</v>
       </c>
       <c r="I9" s="2">
         <v>7</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="2" t="s">
-        <v>503</v>
+        <v>509</v>
       </c>
       <c r="L9" s="2">
         <v>7</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>504</v>
+        <v>510</v>
       </c>
       <c r="O9" s="2">
         <v>7</v>
@@ -6016,7 +5614,7 @@
     </row>
     <row r="10" spans="1:15" ht="15.75">
       <c r="A10" s="2" t="s">
-        <v>505</v>
+        <v>511</v>
       </c>
       <c r="B10" s="2">
         <v>8</v>
@@ -6027,20 +5625,20 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="2" t="s">
-        <v>506</v>
+        <v>512</v>
       </c>
       <c r="I10" s="2">
         <v>8</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="2" t="s">
-        <v>507</v>
+        <v>513</v>
       </c>
       <c r="L10" s="2">
         <v>8</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>508</v>
+        <v>514</v>
       </c>
       <c r="O10" s="2">
         <v>8</v>
@@ -6048,7 +5646,7 @@
     </row>
     <row r="11" spans="1:15" ht="15.75">
       <c r="A11" s="2" t="s">
-        <v>509</v>
+        <v>515</v>
       </c>
       <c r="B11" s="2">
         <v>9</v>
@@ -6059,14 +5657,14 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="2" t="s">
-        <v>510</v>
+        <v>516</v>
       </c>
       <c r="I11" s="2">
         <v>9</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="2" t="s">
-        <v>511</v>
+        <v>517</v>
       </c>
       <c r="L11" s="2">
         <v>9</v>
@@ -6074,7 +5672,7 @@
     </row>
     <row r="12" spans="1:15" ht="15.75">
       <c r="A12" s="2" t="s">
-        <v>512</v>
+        <v>518</v>
       </c>
       <c r="B12" s="2">
         <v>10</v>
@@ -6085,14 +5683,14 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="2" t="s">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="I12" s="2">
         <v>10</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="2" t="s">
-        <v>514</v>
+        <v>520</v>
       </c>
       <c r="L12" s="2">
         <v>10</v>
@@ -6100,7 +5698,7 @@
     </row>
     <row r="13" spans="1:15" ht="15.75">
       <c r="A13" s="2" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="B13" s="2">
         <v>11</v>
@@ -6111,14 +5709,14 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="2" t="s">
-        <v>516</v>
+        <v>522</v>
       </c>
       <c r="I13" s="2">
         <v>11</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="2" t="s">
-        <v>517</v>
+        <v>523</v>
       </c>
       <c r="L13" s="2">
         <v>11</v>
@@ -6126,7 +5724,7 @@
     </row>
     <row r="14" spans="1:15" ht="15.75">
       <c r="A14" s="2" t="s">
-        <v>518</v>
+        <v>524</v>
       </c>
       <c r="B14" s="2">
         <v>12</v>
@@ -6137,14 +5735,14 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="2" t="s">
-        <v>519</v>
+        <v>525</v>
       </c>
       <c r="I14" s="2">
         <v>12</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="2" t="s">
-        <v>520</v>
+        <v>526</v>
       </c>
       <c r="L14" s="2">
         <v>12</v>
@@ -6152,7 +5750,7 @@
     </row>
     <row r="15" spans="1:15" ht="15.75">
       <c r="A15" s="2" t="s">
-        <v>521</v>
+        <v>527</v>
       </c>
       <c r="B15" s="2">
         <v>13</v>
@@ -6163,14 +5761,14 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="2" t="s">
-        <v>522</v>
+        <v>528</v>
       </c>
       <c r="I15" s="2">
         <v>13</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="2" t="s">
-        <v>523</v>
+        <v>529</v>
       </c>
       <c r="L15" s="2">
         <v>13</v>
@@ -6178,7 +5776,7 @@
     </row>
     <row r="16" spans="1:15" ht="15.75">
       <c r="A16" s="2" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B16" s="2">
         <v>14</v>
@@ -6189,22 +5787,22 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="2" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="I16" s="2">
         <v>14</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="2" t="s">
-        <v>526</v>
+        <v>532</v>
       </c>
       <c r="L16" s="2">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="15.75">
+    <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="2" t="s">
-        <v>527</v>
+        <v>533</v>
       </c>
       <c r="B17" s="2">
         <v>15</v>
@@ -6215,7 +5813,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="2" t="s">
-        <v>528</v>
+        <v>534</v>
       </c>
       <c r="I17" s="2">
         <v>15</v>
@@ -6224,9 +5822,9 @@
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
     </row>
-    <row r="18" spans="1:15" ht="15.75">
+    <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="2" t="s">
-        <v>529</v>
+        <v>535</v>
       </c>
       <c r="B18" s="2">
         <v>16</v>
@@ -6242,9 +5840,9 @@
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:15" ht="15.75">
+    <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="2" t="s">
-        <v>530</v>
+        <v>536</v>
       </c>
       <c r="B19" s="2">
         <v>17</v>
@@ -6260,9 +5858,9 @@
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
     </row>
-    <row r="20" spans="1:15" ht="15.75">
+    <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="2" t="s">
-        <v>531</v>
+        <v>537</v>
       </c>
       <c r="B20" s="2">
         <v>18</v>
@@ -6278,9 +5876,9 @@
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
     </row>
-    <row r="21" spans="1:15" ht="15.75">
+    <row r="21" spans="1:12" ht="15.75">
       <c r="A21" s="2" t="s">
-        <v>532</v>
+        <v>538</v>
       </c>
       <c r="B21" s="2">
         <v>19</v>

</xml_diff>

<commit_message>
Super user registro evento
</commit_message>
<xml_diff>
--- a/MyProject2/Content/Excels/Socios.xlsx
+++ b/MyProject2/Content/Excels/Socios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEFB28E2-D20F-4C55-9680-D2CAC9012687}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7F19552-3D5E-4E3F-8BBF-482437853A3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="539">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="540">
   <si>
     <t>Nomre y apellidos</t>
   </si>
@@ -1527,16 +1527,19 @@
     <t>Descuento</t>
   </si>
   <si>
+    <t>ivananfruns1</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>user4</t>
+  </si>
+  <si>
     <t>user1</t>
-  </si>
-  <si>
-    <t>user2</t>
-  </si>
-  <si>
-    <t>user3</t>
-  </si>
-  <si>
-    <t>user4</t>
   </si>
   <si>
     <t>Tipos de empresas</t>
@@ -5214,10 +5217,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C876676D-DD75-4785-895D-73121CF7C510}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5264,6 +5267,14 @@
       </c>
       <c r="B5" s="9">
         <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="8" t="s">
+        <v>466</v>
+      </c>
+      <c r="B6" s="9">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -5290,43 +5301,43 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75">
       <c r="A1" s="3" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>468</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>467</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="6" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="J1" s="4"/>
       <c r="K1" s="7" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75">
       <c r="A2" s="2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -5334,27 +5345,27 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="I2" s="2">
         <v>0</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="L2" s="2">
         <v>0</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="O2" s="2">
         <v>0</v>
@@ -5362,7 +5373,7 @@
     </row>
     <row r="3" spans="1:15" ht="15.75">
       <c r="A3" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -5370,27 +5381,27 @@
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="2" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="2" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="I3" s="2">
         <v>1</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="2" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="L3" s="2">
         <v>1</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="O3" s="2">
         <v>1</v>
@@ -5398,7 +5409,7 @@
     </row>
     <row r="4" spans="1:15" ht="15.75">
       <c r="A4" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B4" s="2">
         <v>2</v>
@@ -5406,27 +5417,27 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="F4" s="2">
         <v>2</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="I4" s="2">
         <v>2</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="L4" s="2">
         <v>2</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="O4" s="2">
         <v>2</v>
@@ -5434,7 +5445,7 @@
     </row>
     <row r="5" spans="1:15" ht="15.75">
       <c r="A5" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B5" s="2">
         <v>3</v>
@@ -5442,27 +5453,27 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="F5" s="2">
         <v>3</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="2" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="I5" s="2">
         <v>3</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="L5" s="2">
         <v>3</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="O5" s="2">
         <v>3</v>
@@ -5470,7 +5481,7 @@
     </row>
     <row r="6" spans="1:15" ht="15.75">
       <c r="A6" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B6" s="2">
         <v>4</v>
@@ -5478,27 +5489,27 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="F6" s="2">
         <v>4</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="I6" s="2">
         <v>4</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="L6" s="2">
         <v>4</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="O6" s="2">
         <v>4</v>
@@ -5506,7 +5517,7 @@
     </row>
     <row r="7" spans="1:15" ht="15.75">
       <c r="A7" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B7" s="2">
         <v>5</v>
@@ -5514,27 +5525,27 @@
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="F7" s="2">
         <v>5</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="I7" s="2">
         <v>5</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="L7" s="2">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="O7" s="2">
         <v>5</v>
@@ -5542,7 +5553,7 @@
     </row>
     <row r="8" spans="1:15" ht="15.75">
       <c r="A8" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B8" s="2">
         <v>6</v>
@@ -5550,27 +5561,27 @@
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="F8" s="2">
         <v>6</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="2" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="I8" s="2">
         <v>6</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="L8" s="2">
         <v>6</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="O8" s="2">
         <v>6</v>
@@ -5578,7 +5589,7 @@
     </row>
     <row r="9" spans="1:15" ht="15.75">
       <c r="A9" s="2" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B9" s="2">
         <v>7</v>
@@ -5586,27 +5597,27 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="F9" s="2">
         <v>7</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="I9" s="2">
         <v>7</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="L9" s="2">
         <v>7</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="O9" s="2">
         <v>7</v>
@@ -5614,7 +5625,7 @@
     </row>
     <row r="10" spans="1:15" ht="15.75">
       <c r="A10" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B10" s="2">
         <v>8</v>
@@ -5625,20 +5636,20 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="I10" s="2">
         <v>8</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="L10" s="2">
         <v>8</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="O10" s="2">
         <v>8</v>
@@ -5646,7 +5657,7 @@
     </row>
     <row r="11" spans="1:15" ht="15.75">
       <c r="A11" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B11" s="2">
         <v>9</v>
@@ -5657,14 +5668,14 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="I11" s="2">
         <v>9</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="L11" s="2">
         <v>9</v>
@@ -5672,7 +5683,7 @@
     </row>
     <row r="12" spans="1:15" ht="15.75">
       <c r="A12" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B12" s="2">
         <v>10</v>
@@ -5683,14 +5694,14 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="I12" s="2">
         <v>10</v>
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="L12" s="2">
         <v>10</v>
@@ -5698,7 +5709,7 @@
     </row>
     <row r="13" spans="1:15" ht="15.75">
       <c r="A13" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B13" s="2">
         <v>11</v>
@@ -5709,14 +5720,14 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="I13" s="2">
         <v>11</v>
       </c>
       <c r="J13" s="4"/>
       <c r="K13" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="L13" s="2">
         <v>11</v>
@@ -5724,7 +5735,7 @@
     </row>
     <row r="14" spans="1:15" ht="15.75">
       <c r="A14" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="B14" s="2">
         <v>12</v>
@@ -5735,14 +5746,14 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="2" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="I14" s="2">
         <v>12</v>
       </c>
       <c r="J14" s="4"/>
       <c r="K14" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="L14" s="2">
         <v>12</v>
@@ -5750,7 +5761,7 @@
     </row>
     <row r="15" spans="1:15" ht="15.75">
       <c r="A15" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B15" s="2">
         <v>13</v>
@@ -5761,14 +5772,14 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="I15" s="2">
         <v>13</v>
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="L15" s="2">
         <v>13</v>
@@ -5776,7 +5787,7 @@
     </row>
     <row r="16" spans="1:15" ht="15.75">
       <c r="A16" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B16" s="2">
         <v>14</v>
@@ -5787,14 +5798,14 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="I16" s="2">
         <v>14</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="L16" s="2">
         <v>14</v>
@@ -5802,7 +5813,7 @@
     </row>
     <row r="17" spans="1:12" ht="15.75">
       <c r="A17" s="2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B17" s="2">
         <v>15</v>
@@ -5813,7 +5824,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="I17" s="2">
         <v>15</v>
@@ -5824,7 +5835,7 @@
     </row>
     <row r="18" spans="1:12" ht="15.75">
       <c r="A18" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="B18" s="2">
         <v>16</v>
@@ -5842,7 +5853,7 @@
     </row>
     <row r="19" spans="1:12" ht="15.75">
       <c r="A19" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="B19" s="2">
         <v>17</v>
@@ -5860,7 +5871,7 @@
     </row>
     <row r="20" spans="1:12" ht="15.75">
       <c r="A20" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B20" s="2">
         <v>18</v>
@@ -5878,7 +5889,7 @@
     </row>
     <row r="21" spans="1:12" ht="15.75">
       <c r="A21" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B21" s="2">
         <v>19</v>

</xml_diff>